<commit_message>
checkpoint for stats output from agent for multiple runs
</commit_message>
<xml_diff>
--- a/CSCI446_Project2_WumpusWorld/references/statistics/AgentRunStatistics.xlsx
+++ b/CSCI446_Project2_WumpusWorld/references/statistics/AgentRunStatistics.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="16">
   <si>
     <t>Map Size: 5x5</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t># Decisions Made</t>
+  </si>
+  <si>
+    <t>Score</t>
   </si>
 </sst>
 </file>
@@ -151,7 +154,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -167,6 +170,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1175,10 +1181,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G114"/>
+  <dimension ref="A1:H114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,20 +1196,22 @@
     <col min="5" max="5" width="18.75" customWidth="1"/>
     <col min="6" max="6" width="23.5" customWidth="1"/>
     <col min="7" max="7" width="15.25" customWidth="1"/>
+    <col min="8" max="8" width="12.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1225,137 +1233,123 @@
       <c r="G2" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>300</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
@@ -1377,119 +1371,123 @@
       <c r="G25" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="3" t="s">
+    <row r="47" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-    </row>
-    <row r="48" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>1</v>
       </c>
@@ -1510,6 +1508,9 @@
       </c>
       <c r="G48" s="6" t="s">
         <v>7</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
@@ -1592,38 +1593,39 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="3" t="s">
+    <row r="70" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A70" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
-    </row>
-    <row r="71" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="7"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="7"/>
+      <c r="E70" s="7"/>
+      <c r="F70" s="7"/>
+      <c r="G70" s="7"/>
+      <c r="H70" s="7"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>1</v>
       </c>
@@ -1645,119 +1647,123 @@
       <c r="G71" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H71" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>16</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="3" t="s">
+    <row r="93" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A93" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B93" s="3"/>
-      <c r="C93" s="3"/>
-      <c r="D93" s="3"/>
-      <c r="E93" s="3"/>
-      <c r="F93" s="3"/>
-      <c r="G93" s="3"/>
-    </row>
-    <row r="94" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B93" s="7"/>
+      <c r="C93" s="7"/>
+      <c r="D93" s="7"/>
+      <c r="E93" s="7"/>
+      <c r="F93" s="7"/>
+      <c r="G93" s="7"/>
+      <c r="H93" s="7"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>1</v>
       </c>
@@ -1779,13 +1785,16 @@
       <c r="G94" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H94" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>2</v>
       </c>
@@ -1882,11 +1891,11 @@
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A24:G24"/>
-    <mergeCell ref="A47:G47"/>
-    <mergeCell ref="A70:G70"/>
-    <mergeCell ref="A93:G93"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A93:H93"/>
+    <mergeCell ref="A70:H70"/>
+    <mergeCell ref="A47:H47"/>
+    <mergeCell ref="A24:H24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Everything but wumpus kills generating as stats
</commit_message>
<xml_diff>
--- a/CSCI446_Project2_WumpusWorld/references/statistics/AgentRunStatistics.xlsx
+++ b/CSCI446_Project2_WumpusWorld/references/statistics/AgentRunStatistics.xlsx
@@ -1184,7 +1184,7 @@
   <dimension ref="A1:H114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1241,100 +1241,520 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>996</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>7</v>
+      </c>
+      <c r="H4">
+        <v>993</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>998</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>14</v>
+      </c>
+      <c r="H6">
+        <v>-22</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
+      </c>
+      <c r="B7">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>15</v>
+      </c>
+      <c r="H7">
+        <v>-22</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>-3</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
+      <c r="B9">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>19</v>
+      </c>
+      <c r="H9">
+        <v>-28</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>994</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>-8</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>5</v>
+      </c>
+      <c r="H12">
+        <v>995</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+      <c r="H13">
+        <v>985</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
+      <c r="B14">
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>18</v>
+      </c>
+      <c r="H14">
+        <v>-24</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
+      <c r="B15">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>17</v>
+      </c>
+      <c r="H15">
+        <v>978</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>14</v>
+      </c>
+      <c r="H16">
+        <v>979</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
+      <c r="B17">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>12</v>
+      </c>
+      <c r="H17">
+        <v>982</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>-3</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
+      <c r="H19">
+        <v>996</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>7</v>
+      </c>
+      <c r="H20">
+        <v>988</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>-3</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
+      </c>
+      <c r="B22">
+        <v>13</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>12</v>
+      </c>
+      <c r="H22">
+        <v>-19</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fixed gold being placed in cell 0,0
</commit_message>
<xml_diff>
--- a/CSCI446_Project2_WumpusWorld/references/statistics/AgentRunStatistics.xlsx
+++ b/CSCI446_Project2_WumpusWorld/references/statistics/AgentRunStatistics.xlsx
@@ -154,11 +154,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -166,14 +172,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -469,54 +472,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
     </row>
     <row r="2" spans="1:21" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -614,52 +617,52 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
-      <c r="T10" s="4"/>
-      <c r="U10" s="4"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
     </row>
     <row r="11" spans="1:21" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
     </row>
     <row r="12" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -757,52 +760,52 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
-      <c r="U19" s="4"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
     </row>
     <row r="20" spans="1:21" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
     </row>
     <row r="21" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -900,52 +903,52 @@
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="4"/>
-      <c r="T28" s="4"/>
-      <c r="U28" s="4"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="6"/>
+      <c r="U28" s="6"/>
     </row>
     <row r="29" spans="1:21" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-      <c r="R29" s="3"/>
-      <c r="S29" s="3"/>
-      <c r="T29" s="3"/>
-      <c r="U29" s="3"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
     </row>
     <row r="30" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -1043,29 +1046,29 @@
       </c>
     </row>
     <row r="38" spans="1:21" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
-      <c r="O38" s="3"/>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="3"/>
-      <c r="R38" s="3"/>
-      <c r="S38" s="3"/>
-      <c r="T38" s="3"/>
-      <c r="U38" s="3"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="5"/>
+      <c r="S38" s="5"/>
+      <c r="T38" s="5"/>
+      <c r="U38" s="5"/>
     </row>
     <row r="39" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
@@ -1164,15 +1167,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A38:U38"/>
+    <mergeCell ref="A10:U10"/>
+    <mergeCell ref="A19:U19"/>
+    <mergeCell ref="A28:U28"/>
     <mergeCell ref="A1:U1"/>
     <mergeCell ref="A2:U2"/>
     <mergeCell ref="A11:U11"/>
     <mergeCell ref="A20:U20"/>
     <mergeCell ref="A29:U29"/>
-    <mergeCell ref="A38:U38"/>
-    <mergeCell ref="A10:U10"/>
-    <mergeCell ref="A19:U19"/>
-    <mergeCell ref="A28:U28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1184,7 +1187,7 @@
   <dimension ref="A1:H114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1215,25 +1218,25 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="6" t="s">
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1241,103 +1244,103 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3">
-        <v>996</v>
+      <c r="B3" s="8">
+        <v>12</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8">
+        <v>12</v>
+      </c>
+      <c r="H3" s="8">
+        <v>984</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>7</v>
-      </c>
-      <c r="H4">
-        <v>993</v>
+      <c r="B4" s="8">
+        <v>12</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0</v>
+      </c>
+      <c r="G4" s="8">
+        <v>11</v>
+      </c>
+      <c r="H4" s="8">
+        <v>-17</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>998</v>
+      <c r="B5" s="8">
+        <v>6</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8">
+        <v>5</v>
+      </c>
+      <c r="H5" s="8">
+        <v>-8</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="8">
         <v>15</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
+      <c r="C6" s="8">
+        <v>0</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8">
         <v>14</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="8">
         <v>-22</v>
       </c>
     </row>
@@ -1345,416 +1348,416 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>16</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>15</v>
-      </c>
-      <c r="H7">
-        <v>-22</v>
+      <c r="B7" s="8">
+        <v>11</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0</v>
+      </c>
+      <c r="G7" s="8">
+        <v>10</v>
+      </c>
+      <c r="H7" s="8">
+        <v>-14</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
-      <c r="H8">
-        <v>-3</v>
+      <c r="B8" s="8">
+        <v>21</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="8">
+        <v>21</v>
+      </c>
+      <c r="H8" s="8">
+        <v>974</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>20</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>19</v>
-      </c>
-      <c r="H9">
-        <v>-28</v>
+      <c r="B9" s="8">
+        <v>23</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0</v>
+      </c>
+      <c r="G9" s="8">
+        <v>22</v>
+      </c>
+      <c r="H9" s="8">
+        <v>-26</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>5</v>
-      </c>
-      <c r="H10">
-        <v>994</v>
+      <c r="B10" s="8">
+        <v>13</v>
+      </c>
+      <c r="C10" s="8">
+        <v>1</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0</v>
+      </c>
+      <c r="G10" s="8">
+        <v>13</v>
+      </c>
+      <c r="H10" s="8">
+        <v>981</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>6</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>5</v>
-      </c>
-      <c r="H11">
-        <v>-8</v>
+      <c r="B11" s="8">
+        <v>23</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0</v>
+      </c>
+      <c r="G11" s="8">
+        <v>22</v>
+      </c>
+      <c r="H11" s="8">
+        <v>-29</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12">
-        <v>5</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>5</v>
-      </c>
-      <c r="H12">
-        <v>995</v>
+      <c r="B12" s="8">
+        <v>20</v>
+      </c>
+      <c r="C12" s="8">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0</v>
+      </c>
+      <c r="G12" s="8">
+        <v>20</v>
+      </c>
+      <c r="H12" s="8">
+        <v>968</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13">
-        <v>12</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>12</v>
-      </c>
-      <c r="H13">
-        <v>985</v>
+      <c r="B13" s="8">
+        <v>19</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0</v>
+      </c>
+      <c r="G13" s="8">
+        <v>18</v>
+      </c>
+      <c r="H13" s="8">
+        <v>-26</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14">
-        <v>19</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>18</v>
-      </c>
-      <c r="H14">
-        <v>-24</v>
+      <c r="B14" s="8">
+        <v>11</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0</v>
+      </c>
+      <c r="G14" s="8">
+        <v>10</v>
+      </c>
+      <c r="H14" s="8">
+        <v>-14</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15">
-        <v>17</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>17</v>
-      </c>
-      <c r="H15">
-        <v>978</v>
+      <c r="B15" s="8">
+        <v>6</v>
+      </c>
+      <c r="C15" s="8">
+        <v>1</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0</v>
+      </c>
+      <c r="G15" s="8">
+        <v>6</v>
+      </c>
+      <c r="H15" s="8">
+        <v>994</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16">
-        <v>14</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>14</v>
-      </c>
-      <c r="H16">
-        <v>979</v>
+      <c r="B16" s="8">
+        <v>18</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0</v>
+      </c>
+      <c r="G16" s="8">
+        <v>17</v>
+      </c>
+      <c r="H16" s="8">
+        <v>-24</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17">
-        <v>12</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>12</v>
-      </c>
-      <c r="H17">
-        <v>982</v>
+      <c r="B17" s="8">
+        <v>6</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0</v>
+      </c>
+      <c r="E17" s="8">
+        <v>0</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0</v>
+      </c>
+      <c r="G17" s="8">
+        <v>5</v>
+      </c>
+      <c r="H17" s="8">
+        <v>-8</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18">
-        <v>3</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>2</v>
-      </c>
-      <c r="H18">
-        <v>-3</v>
+      <c r="B18" s="8">
+        <v>7</v>
+      </c>
+      <c r="C18" s="8">
+        <v>1</v>
+      </c>
+      <c r="D18" s="8">
+        <v>0</v>
+      </c>
+      <c r="E18" s="8">
+        <v>0</v>
+      </c>
+      <c r="F18" s="8">
+        <v>0</v>
+      </c>
+      <c r="G18" s="8">
+        <v>7</v>
+      </c>
+      <c r="H18" s="8">
+        <v>990</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19">
-        <v>4</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>4</v>
-      </c>
-      <c r="H19">
-        <v>996</v>
+      <c r="B19" s="8">
+        <v>6</v>
+      </c>
+      <c r="C19" s="8">
+        <v>0</v>
+      </c>
+      <c r="D19" s="8">
+        <v>0</v>
+      </c>
+      <c r="E19" s="8">
+        <v>0</v>
+      </c>
+      <c r="F19" s="8">
+        <v>0</v>
+      </c>
+      <c r="G19" s="8">
+        <v>5</v>
+      </c>
+      <c r="H19" s="8">
+        <v>-8</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20">
-        <v>7</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>7</v>
-      </c>
-      <c r="H20">
-        <v>988</v>
+      <c r="B20" s="8">
+        <v>10</v>
+      </c>
+      <c r="C20" s="8">
+        <v>0</v>
+      </c>
+      <c r="D20" s="8">
+        <v>0</v>
+      </c>
+      <c r="E20" s="8">
+        <v>0</v>
+      </c>
+      <c r="F20" s="8">
+        <v>0</v>
+      </c>
+      <c r="G20" s="8">
+        <v>9</v>
+      </c>
+      <c r="H20" s="8">
+        <v>-15</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21">
-        <v>3</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>2</v>
-      </c>
-      <c r="H21">
-        <v>-3</v>
+      <c r="B21" s="8">
+        <v>10</v>
+      </c>
+      <c r="C21" s="8">
+        <v>1</v>
+      </c>
+      <c r="D21" s="8">
+        <v>0</v>
+      </c>
+      <c r="E21" s="8">
+        <v>0</v>
+      </c>
+      <c r="F21" s="8">
+        <v>0</v>
+      </c>
+      <c r="G21" s="8">
+        <v>10</v>
+      </c>
+      <c r="H21" s="8">
+        <v>990</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22">
-        <v>13</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>12</v>
-      </c>
-      <c r="H22">
-        <v>-19</v>
+      <c r="B22" s="8">
+        <v>3</v>
+      </c>
+      <c r="C22" s="8">
+        <v>0</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0</v>
+      </c>
+      <c r="E22" s="8">
+        <v>0</v>
+      </c>
+      <c r="F22" s="8">
+        <v>0</v>
+      </c>
+      <c r="G22" s="8">
+        <v>2</v>
+      </c>
+      <c r="H22" s="8">
+        <v>-3</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1773,25 +1776,25 @@
       <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G25" s="6" t="s">
+      <c r="F25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="H25" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1911,25 +1914,25 @@
       <c r="A48" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D48" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E48" s="6" t="s">
+      <c r="E48" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F48" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G48" s="6" t="s">
+      <c r="F48" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G48" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H48" s="6" t="s">
+      <c r="H48" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2049,25 +2052,25 @@
       <c r="A71" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="B71" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C71" s="6" t="s">
+      <c r="C71" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D71" s="6" t="s">
+      <c r="D71" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E71" s="6" t="s">
+      <c r="E71" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F71" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G71" s="6" t="s">
+      <c r="F71" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G71" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H71" s="6" t="s">
+      <c r="H71" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2187,25 +2190,25 @@
       <c r="A94" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B94" s="6" t="s">
+      <c r="B94" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C94" s="6" t="s">
+      <c r="C94" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D94" s="6" t="s">
+      <c r="D94" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E94" s="6" t="s">
+      <c r="E94" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F94" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G94" s="6" t="s">
+      <c r="F94" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G94" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H94" s="6" t="s">
+      <c r="H94" s="3" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fire arrow and kill wumpus working (stat tracking as well)
</commit_message>
<xml_diff>
--- a/CSCI446_Project2_WumpusWorld/references/statistics/AgentRunStatistics.xlsx
+++ b/CSCI446_Project2_WumpusWorld/references/statistics/AgentRunStatistics.xlsx
@@ -163,8 +163,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -172,11 +172,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -472,29 +472,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
     </row>
     <row r="2" spans="1:21" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -1187,7 +1187,7 @@
   <dimension ref="A1:H114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,16 +1203,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1244,533 +1244,533 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="8">
-        <v>12</v>
-      </c>
-      <c r="C3" s="8">
-        <v>1</v>
-      </c>
-      <c r="D3" s="8">
-        <v>0</v>
-      </c>
-      <c r="E3" s="8">
-        <v>0</v>
-      </c>
-      <c r="F3" s="8">
-        <v>0</v>
-      </c>
-      <c r="G3" s="8">
-        <v>12</v>
-      </c>
-      <c r="H3" s="8">
-        <v>984</v>
+      <c r="B3" s="4">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>6</v>
+      </c>
+      <c r="H3" s="4">
+        <v>-9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="4">
         <v>12</v>
       </c>
-      <c r="C4" s="8">
-        <v>0</v>
-      </c>
-      <c r="D4" s="8">
-        <v>0</v>
-      </c>
-      <c r="E4" s="8">
-        <v>0</v>
-      </c>
-      <c r="F4" s="8">
-        <v>0</v>
-      </c>
-      <c r="G4" s="8">
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
         <v>11</v>
       </c>
-      <c r="H4" s="8">
-        <v>-17</v>
+      <c r="H4" s="4">
+        <v>-16</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="8">
-        <v>6</v>
-      </c>
-      <c r="C5" s="8">
-        <v>0</v>
-      </c>
-      <c r="D5" s="8">
-        <v>0</v>
-      </c>
-      <c r="E5" s="8">
-        <v>0</v>
-      </c>
-      <c r="F5" s="8">
-        <v>0</v>
-      </c>
-      <c r="G5" s="8">
-        <v>5</v>
-      </c>
-      <c r="H5" s="8">
-        <v>-8</v>
+      <c r="B5" s="4">
+        <v>17</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>17</v>
+      </c>
+      <c r="H5" s="4">
+        <v>979</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="8">
-        <v>15</v>
-      </c>
-      <c r="C6" s="8">
-        <v>0</v>
-      </c>
-      <c r="D6" s="8">
-        <v>0</v>
-      </c>
-      <c r="E6" s="8">
-        <v>0</v>
-      </c>
-      <c r="F6" s="8">
-        <v>0</v>
-      </c>
-      <c r="G6" s="8">
-        <v>14</v>
-      </c>
-      <c r="H6" s="8">
-        <v>-22</v>
+      <c r="B6" s="4">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>8</v>
+      </c>
+      <c r="H6" s="4">
+        <v>991</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="8">
-        <v>11</v>
-      </c>
-      <c r="C7" s="8">
-        <v>0</v>
-      </c>
-      <c r="D7" s="8">
-        <v>0</v>
-      </c>
-      <c r="E7" s="8">
-        <v>0</v>
-      </c>
-      <c r="F7" s="8">
-        <v>0</v>
-      </c>
-      <c r="G7" s="8">
+      <c r="B7" s="4">
         <v>10</v>
       </c>
-      <c r="H7" s="8">
-        <v>-14</v>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>9</v>
+      </c>
+      <c r="H7" s="4">
+        <v>-16</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="8">
-        <v>21</v>
-      </c>
-      <c r="C8" s="8">
-        <v>1</v>
-      </c>
-      <c r="D8" s="8">
-        <v>0</v>
-      </c>
-      <c r="E8" s="8">
-        <v>0</v>
-      </c>
-      <c r="F8" s="8">
-        <v>0</v>
-      </c>
-      <c r="G8" s="8">
-        <v>21</v>
-      </c>
-      <c r="H8" s="8">
-        <v>974</v>
+      <c r="B8" s="4">
+        <v>16</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>16</v>
+      </c>
+      <c r="H8" s="4">
+        <v>979</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="8">
-        <v>23</v>
-      </c>
-      <c r="C9" s="8">
-        <v>0</v>
-      </c>
-      <c r="D9" s="8">
-        <v>0</v>
-      </c>
-      <c r="E9" s="8">
-        <v>0</v>
-      </c>
-      <c r="F9" s="8">
-        <v>0</v>
-      </c>
-      <c r="G9" s="8">
-        <v>22</v>
-      </c>
-      <c r="H9" s="8">
-        <v>-26</v>
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="8">
-        <v>13</v>
-      </c>
-      <c r="C10" s="8">
-        <v>1</v>
-      </c>
-      <c r="D10" s="8">
-        <v>0</v>
-      </c>
-      <c r="E10" s="8">
-        <v>0</v>
-      </c>
-      <c r="F10" s="8">
-        <v>0</v>
-      </c>
-      <c r="G10" s="8">
-        <v>13</v>
-      </c>
-      <c r="H10" s="8">
-        <v>981</v>
+      <c r="B10" s="4">
+        <v>9</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>9</v>
+      </c>
+      <c r="H10" s="4">
+        <v>990</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="8">
-        <v>23</v>
-      </c>
-      <c r="C11" s="8">
-        <v>0</v>
-      </c>
-      <c r="D11" s="8">
-        <v>0</v>
-      </c>
-      <c r="E11" s="8">
-        <v>0</v>
-      </c>
-      <c r="F11" s="8">
-        <v>0</v>
-      </c>
-      <c r="G11" s="8">
-        <v>22</v>
-      </c>
-      <c r="H11" s="8">
-        <v>-29</v>
+      <c r="B11" s="4">
+        <v>15</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>14</v>
+      </c>
+      <c r="H11" s="4">
+        <v>-19</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="8">
-        <v>20</v>
-      </c>
-      <c r="C12" s="8">
-        <v>1</v>
-      </c>
-      <c r="D12" s="8">
-        <v>0</v>
-      </c>
-      <c r="E12" s="8">
-        <v>0</v>
-      </c>
-      <c r="F12" s="8">
-        <v>0</v>
-      </c>
-      <c r="G12" s="8">
-        <v>20</v>
-      </c>
-      <c r="H12" s="8">
-        <v>968</v>
+      <c r="B12" s="4">
+        <v>9</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>9</v>
+      </c>
+      <c r="H12" s="4">
+        <v>987</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="8">
-        <v>19</v>
-      </c>
-      <c r="C13" s="8">
-        <v>0</v>
-      </c>
-      <c r="D13" s="8">
-        <v>0</v>
-      </c>
-      <c r="E13" s="8">
-        <v>0</v>
-      </c>
-      <c r="F13" s="8">
-        <v>0</v>
-      </c>
-      <c r="G13" s="8">
-        <v>18</v>
-      </c>
-      <c r="H13" s="8">
-        <v>-26</v>
+      <c r="B13" s="4">
+        <v>6</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>5</v>
+      </c>
+      <c r="H13" s="4">
+        <v>-8</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="8">
-        <v>11</v>
-      </c>
-      <c r="C14" s="8">
-        <v>0</v>
-      </c>
-      <c r="D14" s="8">
-        <v>0</v>
-      </c>
-      <c r="E14" s="8">
-        <v>0</v>
-      </c>
-      <c r="F14" s="8">
-        <v>0</v>
-      </c>
-      <c r="G14" s="8">
-        <v>10</v>
-      </c>
-      <c r="H14" s="8">
-        <v>-14</v>
+      <c r="B14" s="4">
+        <v>12</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>12</v>
+      </c>
+      <c r="H14" s="4">
+        <v>984</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="8">
-        <v>6</v>
-      </c>
-      <c r="C15" s="8">
-        <v>1</v>
-      </c>
-      <c r="D15" s="8">
-        <v>0</v>
-      </c>
-      <c r="E15" s="8">
-        <v>0</v>
-      </c>
-      <c r="F15" s="8">
-        <v>0</v>
-      </c>
-      <c r="G15" s="8">
-        <v>6</v>
-      </c>
-      <c r="H15" s="8">
-        <v>994</v>
+      <c r="B15" s="4">
+        <v>3</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>2</v>
+      </c>
+      <c r="H15" s="4">
+        <v>-3</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="8">
-        <v>18</v>
-      </c>
-      <c r="C16" s="8">
-        <v>0</v>
-      </c>
-      <c r="D16" s="8">
-        <v>0</v>
-      </c>
-      <c r="E16" s="8">
-        <v>0</v>
-      </c>
-      <c r="F16" s="8">
-        <v>0</v>
-      </c>
-      <c r="G16" s="8">
-        <v>17</v>
-      </c>
-      <c r="H16" s="8">
-        <v>-24</v>
+      <c r="B16" s="4">
+        <v>12</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>11</v>
+      </c>
+      <c r="H16" s="4">
+        <v>-18</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="8">
-        <v>6</v>
-      </c>
-      <c r="C17" s="8">
-        <v>0</v>
-      </c>
-      <c r="D17" s="8">
-        <v>0</v>
-      </c>
-      <c r="E17" s="8">
-        <v>0</v>
-      </c>
-      <c r="F17" s="8">
-        <v>0</v>
-      </c>
-      <c r="G17" s="8">
-        <v>5</v>
-      </c>
-      <c r="H17" s="8">
-        <v>-8</v>
+      <c r="B17" s="4">
+        <v>11</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>10</v>
+      </c>
+      <c r="H17" s="4">
+        <v>-13</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="8">
-        <v>7</v>
-      </c>
-      <c r="C18" s="8">
-        <v>1</v>
-      </c>
-      <c r="D18" s="8">
-        <v>0</v>
-      </c>
-      <c r="E18" s="8">
-        <v>0</v>
-      </c>
-      <c r="F18" s="8">
-        <v>0</v>
-      </c>
-      <c r="G18" s="8">
-        <v>7</v>
-      </c>
-      <c r="H18" s="8">
-        <v>990</v>
+      <c r="B18" s="4">
+        <v>11</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>11</v>
+      </c>
+      <c r="H18" s="4">
+        <v>987</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="8">
-        <v>6</v>
-      </c>
-      <c r="C19" s="8">
-        <v>0</v>
-      </c>
-      <c r="D19" s="8">
-        <v>0</v>
-      </c>
-      <c r="E19" s="8">
-        <v>0</v>
-      </c>
-      <c r="F19" s="8">
-        <v>0</v>
-      </c>
-      <c r="G19" s="8">
-        <v>5</v>
-      </c>
-      <c r="H19" s="8">
-        <v>-8</v>
+      <c r="B19" s="4">
+        <v>4</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4">
+        <v>4</v>
+      </c>
+      <c r="H19" s="4">
+        <v>996</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="4">
         <v>10</v>
       </c>
-      <c r="C20" s="8">
-        <v>0</v>
-      </c>
-      <c r="D20" s="8">
-        <v>0</v>
-      </c>
-      <c r="E20" s="8">
-        <v>0</v>
-      </c>
-      <c r="F20" s="8">
-        <v>0</v>
-      </c>
-      <c r="G20" s="8">
-        <v>9</v>
-      </c>
-      <c r="H20" s="8">
-        <v>-15</v>
+      <c r="C20" s="4">
+        <v>1</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="4">
+        <v>10</v>
+      </c>
+      <c r="H20" s="4">
+        <v>989</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="8">
-        <v>10</v>
-      </c>
-      <c r="C21" s="8">
-        <v>1</v>
-      </c>
-      <c r="D21" s="8">
-        <v>0</v>
-      </c>
-      <c r="E21" s="8">
-        <v>0</v>
-      </c>
-      <c r="F21" s="8">
-        <v>0</v>
-      </c>
-      <c r="G21" s="8">
-        <v>10</v>
-      </c>
-      <c r="H21" s="8">
-        <v>990</v>
+      <c r="B21" s="4">
+        <v>22</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0</v>
+      </c>
+      <c r="G21" s="4">
+        <v>22</v>
+      </c>
+      <c r="H21" s="4">
+        <v>980</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="8">
-        <v>3</v>
-      </c>
-      <c r="C22" s="8">
-        <v>0</v>
-      </c>
-      <c r="D22" s="8">
-        <v>0</v>
-      </c>
-      <c r="E22" s="8">
-        <v>0</v>
-      </c>
-      <c r="F22" s="8">
-        <v>0</v>
-      </c>
-      <c r="G22" s="8">
-        <v>2</v>
-      </c>
-      <c r="H22" s="8">
-        <v>-3</v>
+      <c r="B22" s="4">
+        <v>14</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0</v>
+      </c>
+      <c r="G22" s="4">
+        <v>13</v>
+      </c>
+      <c r="H22" s="4">
+        <v>-20</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -1899,16 +1899,16 @@
       </c>
     </row>
     <row r="47" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
@@ -2037,16 +2037,16 @@
       </c>
     </row>
     <row r="70" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A70" s="7" t="s">
+      <c r="A70" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B70" s="7"/>
-      <c r="C70" s="7"/>
-      <c r="D70" s="7"/>
-      <c r="E70" s="7"/>
-      <c r="F70" s="7"/>
-      <c r="G70" s="7"/>
-      <c r="H70" s="7"/>
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+      <c r="G70" s="8"/>
+      <c r="H70" s="8"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
@@ -2175,16 +2175,16 @@
       </c>
     </row>
     <row r="93" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A93" s="7" t="s">
+      <c r="A93" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B93" s="7"/>
-      <c r="C93" s="7"/>
-      <c r="D93" s="7"/>
-      <c r="E93" s="7"/>
-      <c r="F93" s="7"/>
-      <c r="G93" s="7"/>
-      <c r="H93" s="7"/>
+      <c r="B93" s="8"/>
+      <c r="C93" s="8"/>
+      <c r="D93" s="8"/>
+      <c r="E93" s="8"/>
+      <c r="F93" s="8"/>
+      <c r="G93" s="8"/>
+      <c r="H93" s="8"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">

</xml_diff>

<commit_message>
Moving to room fixed. This is an intial completed version of the kb agent
</commit_message>
<xml_diff>
--- a/CSCI446_Project2_WumpusWorld/references/statistics/AgentRunStatistics.xlsx
+++ b/CSCI446_Project2_WumpusWorld/references/statistics/AgentRunStatistics.xlsx
@@ -1187,7 +1187,7 @@
   <dimension ref="A1:H114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1245,10 +1245,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="C3" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="4">
         <v>0</v>
@@ -1260,10 +1260,10 @@
         <v>0</v>
       </c>
       <c r="G3" s="4">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="H3" s="4">
-        <v>-9</v>
+        <v>973</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1271,10 +1271,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="4">
-        <v>12</v>
+        <v>108</v>
       </c>
       <c r="C4" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="4">
         <v>0</v>
@@ -1286,10 +1286,10 @@
         <v>0</v>
       </c>
       <c r="G4" s="4">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="H4" s="4">
-        <v>-16</v>
+        <v>951</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1297,10 +1297,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C5" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="4">
         <v>0</v>
@@ -1312,10 +1312,10 @@
         <v>0</v>
       </c>
       <c r="G5" s="4">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="H5" s="4">
-        <v>979</v>
+        <v>-16</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1323,7 +1323,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
@@ -1338,10 +1338,10 @@
         <v>0</v>
       </c>
       <c r="G6" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H6" s="4">
-        <v>991</v>
+        <v>980</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1349,13 +1349,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="4">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="C7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="4">
         <v>0</v>
@@ -1364,10 +1364,10 @@
         <v>0</v>
       </c>
       <c r="G7" s="4">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="H7" s="4">
-        <v>-16</v>
+        <v>957</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1375,13 +1375,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="4">
-        <v>16</v>
+        <v>112</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
       </c>
       <c r="D8" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E8" s="4">
         <v>0</v>
@@ -1390,10 +1390,10 @@
         <v>0</v>
       </c>
       <c r="G8" s="4">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="H8" s="4">
-        <v>979</v>
+        <v>967</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1401,10 +1401,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="4">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="C9" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="4">
         <v>0</v>
@@ -1416,10 +1416,10 @@
         <v>0</v>
       </c>
       <c r="G9" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H9" s="4">
-        <v>0</v>
+        <v>967</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1427,7 +1427,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="4">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
@@ -1442,10 +1442,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="4">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H10" s="4">
-        <v>990</v>
+        <v>974</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1453,10 +1453,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="4">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="C11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="4">
         <v>0</v>
@@ -1468,10 +1468,10 @@
         <v>0</v>
       </c>
       <c r="G11" s="4">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="H11" s="4">
-        <v>-19</v>
+        <v>976</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1479,10 +1479,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="4">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C12" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="4">
         <v>0</v>
@@ -1494,10 +1494,10 @@
         <v>0</v>
       </c>
       <c r="G12" s="4">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H12" s="4">
-        <v>987</v>
+        <v>-24</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1505,7 +1505,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="4">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C13" s="4">
         <v>0</v>
@@ -1520,10 +1520,10 @@
         <v>0</v>
       </c>
       <c r="G13" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H13" s="4">
-        <v>-8</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1531,13 +1531,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="4">
-        <v>12</v>
+        <v>123</v>
       </c>
       <c r="C14" s="4">
         <v>1</v>
       </c>
       <c r="D14" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="4">
         <v>0</v>
@@ -1546,10 +1546,10 @@
         <v>0</v>
       </c>
       <c r="G14" s="4">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="H14" s="4">
-        <v>984</v>
+        <v>958</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1557,10 +1557,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="4">
-        <v>3</v>
+        <v>98</v>
       </c>
       <c r="C15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="4">
         <v>0</v>
@@ -1572,10 +1572,10 @@
         <v>0</v>
       </c>
       <c r="G15" s="4">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="H15" s="4">
-        <v>-3</v>
+        <v>962</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1583,7 +1583,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="4">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="C16" s="4">
         <v>0</v>
@@ -1598,10 +1598,10 @@
         <v>0</v>
       </c>
       <c r="G16" s="4">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="H16" s="4">
-        <v>-18</v>
+        <v>-44</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1609,7 +1609,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="4">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="C17" s="4">
         <v>0</v>
@@ -1627,7 +1627,7 @@
         <v>10</v>
       </c>
       <c r="H17" s="4">
-        <v>-13</v>
+        <v>-26</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1635,10 +1635,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="4">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C18" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="4">
         <v>0</v>
@@ -1650,10 +1650,10 @@
         <v>0</v>
       </c>
       <c r="G18" s="4">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="H18" s="4">
-        <v>987</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1661,10 +1661,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="4">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C19" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" s="4">
         <v>0</v>
@@ -1676,10 +1676,10 @@
         <v>0</v>
       </c>
       <c r="G19" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H19" s="4">
-        <v>996</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1687,10 +1687,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="4">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="C20" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" s="4">
         <v>0</v>
@@ -1702,10 +1702,10 @@
         <v>0</v>
       </c>
       <c r="G20" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H20" s="4">
-        <v>989</v>
+        <v>-36</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1713,13 +1713,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="4">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="C21" s="4">
         <v>1</v>
       </c>
       <c r="D21" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" s="4">
         <v>0</v>
@@ -1728,10 +1728,10 @@
         <v>0</v>
       </c>
       <c r="G21" s="4">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="H21" s="4">
-        <v>980</v>
+        <v>978</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1739,13 +1739,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="4">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="C22" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="4">
         <v>0</v>
@@ -1754,10 +1754,10 @@
         <v>0</v>
       </c>
       <c r="G22" s="4">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="H22" s="4">
-        <v>-20</v>
+        <v>967</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
All runs up to size 25x25 completed. Run_Results added and excel spreadsheet updated
</commit_message>
<xml_diff>
--- a/CSCI446_Project2_WumpusWorld/references/statistics/AgentRunStatistics.xlsx
+++ b/CSCI446_Project2_WumpusWorld/references/statistics/AgentRunStatistics.xlsx
@@ -154,7 +154,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -165,6 +165,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -472,54 +475,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
     </row>
     <row r="2" spans="1:21" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -617,52 +620,52 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
     </row>
     <row r="11" spans="1:21" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
-      <c r="U11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
     </row>
     <row r="12" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -760,52 +763,52 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
-      <c r="S19" s="6"/>
-      <c r="T19" s="6"/>
-      <c r="U19" s="6"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
     </row>
     <row r="20" spans="1:21" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="5"/>
-      <c r="T20" s="5"/>
-      <c r="U20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
     </row>
     <row r="21" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -903,52 +906,52 @@
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="6"/>
-      <c r="R28" s="6"/>
-      <c r="S28" s="6"/>
-      <c r="T28" s="6"/>
-      <c r="U28" s="6"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="7"/>
+      <c r="U28" s="7"/>
     </row>
     <row r="29" spans="1:21" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
-      <c r="S29" s="5"/>
-      <c r="T29" s="5"/>
-      <c r="U29" s="5"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="6"/>
+      <c r="U29" s="6"/>
     </row>
     <row r="30" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -1046,29 +1049,29 @@
       </c>
     </row>
     <row r="38" spans="1:21" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="5"/>
-      <c r="L38" s="5"/>
-      <c r="M38" s="5"/>
-      <c r="N38" s="5"/>
-      <c r="O38" s="5"/>
-      <c r="P38" s="5"/>
-      <c r="Q38" s="5"/>
-      <c r="R38" s="5"/>
-      <c r="S38" s="5"/>
-      <c r="T38" s="5"/>
-      <c r="U38" s="5"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="6"/>
+      <c r="P38" s="6"/>
+      <c r="Q38" s="6"/>
+      <c r="R38" s="6"/>
+      <c r="S38" s="6"/>
+      <c r="T38" s="6"/>
+      <c r="U38" s="6"/>
     </row>
     <row r="39" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
@@ -1186,8 +1189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,16 +1206,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1635,10 +1638,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="4">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="C18" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="4">
         <v>0</v>
@@ -1650,10 +1653,10 @@
         <v>0</v>
       </c>
       <c r="G18" s="4">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H18" s="4">
-        <v>0</v>
+        <v>976</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1761,16 +1764,16 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -1801,114 +1804,534 @@
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>1</v>
+      </c>
+      <c r="B26" s="4">
+        <v>50</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0</v>
+      </c>
+      <c r="E26" s="4">
+        <v>0</v>
+      </c>
+      <c r="F26" s="4">
+        <v>0</v>
+      </c>
+      <c r="G26" s="4">
+        <v>10</v>
+      </c>
+      <c r="H26" s="4">
+        <v>-28</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>2</v>
       </c>
+      <c r="B27" s="4">
+        <v>69</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0</v>
+      </c>
+      <c r="F27" s="4">
+        <v>0</v>
+      </c>
+      <c r="G27" s="4">
+        <v>13</v>
+      </c>
+      <c r="H27" s="4">
+        <v>-40</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>3</v>
       </c>
+      <c r="B28" s="4">
+        <v>78</v>
+      </c>
+      <c r="C28" s="4">
+        <v>1</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0</v>
+      </c>
+      <c r="F28" s="4">
+        <v>0</v>
+      </c>
+      <c r="G28" s="4">
+        <v>15</v>
+      </c>
+      <c r="H28" s="4">
+        <v>969</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>4</v>
       </c>
+      <c r="B29" s="4">
+        <v>19</v>
+      </c>
+      <c r="C29" s="4">
+        <v>1</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0</v>
+      </c>
+      <c r="E29" s="4">
+        <v>0</v>
+      </c>
+      <c r="F29" s="4">
+        <v>0</v>
+      </c>
+      <c r="G29" s="4">
+        <v>4</v>
+      </c>
+      <c r="H29" s="4">
+        <v>994</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>5</v>
       </c>
+      <c r="B30" s="4">
+        <v>139</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0</v>
+      </c>
+      <c r="D30" s="4">
+        <v>0</v>
+      </c>
+      <c r="E30" s="4">
+        <v>0</v>
+      </c>
+      <c r="F30" s="4">
+        <v>0</v>
+      </c>
+      <c r="G30" s="4">
+        <v>27</v>
+      </c>
+      <c r="H30" s="4">
+        <v>-90</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>6</v>
       </c>
+      <c r="B31" s="4">
+        <v>471</v>
+      </c>
+      <c r="C31" s="4">
+        <v>1</v>
+      </c>
+      <c r="D31" s="4">
+        <v>6</v>
+      </c>
+      <c r="E31" s="4">
+        <v>0</v>
+      </c>
+      <c r="F31" s="4">
+        <v>0</v>
+      </c>
+      <c r="G31" s="4">
+        <v>100</v>
+      </c>
+      <c r="H31" s="4">
+        <v>817</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>7</v>
       </c>
+      <c r="B32" s="4">
+        <v>408</v>
+      </c>
+      <c r="C32" s="4">
+        <v>1</v>
+      </c>
+      <c r="D32" s="4">
+        <v>5</v>
+      </c>
+      <c r="E32" s="4">
+        <v>0</v>
+      </c>
+      <c r="F32" s="4">
+        <v>0</v>
+      </c>
+      <c r="G32" s="4">
+        <v>83</v>
+      </c>
+      <c r="H32" s="4">
+        <v>849</v>
+      </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>8</v>
       </c>
+      <c r="B33" s="4">
+        <v>23</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0</v>
+      </c>
+      <c r="D33" s="4">
+        <v>0</v>
+      </c>
+      <c r="E33" s="4">
+        <v>0</v>
+      </c>
+      <c r="F33" s="4">
+        <v>0</v>
+      </c>
+      <c r="G33" s="4">
+        <v>5</v>
+      </c>
+      <c r="H33" s="4">
+        <v>-16</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>9</v>
       </c>
+      <c r="B34" s="4">
+        <v>43</v>
+      </c>
+      <c r="C34" s="4">
+        <v>1</v>
+      </c>
+      <c r="D34" s="4">
+        <v>0</v>
+      </c>
+      <c r="E34" s="4">
+        <v>0</v>
+      </c>
+      <c r="F34" s="4">
+        <v>0</v>
+      </c>
+      <c r="G34" s="4">
+        <v>8</v>
+      </c>
+      <c r="H34" s="4">
+        <v>982</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>10</v>
       </c>
+      <c r="B35" s="4">
+        <v>101</v>
+      </c>
+      <c r="C35" s="4">
+        <v>0</v>
+      </c>
+      <c r="D35" s="4">
+        <v>0</v>
+      </c>
+      <c r="E35" s="4">
+        <v>0</v>
+      </c>
+      <c r="F35" s="4">
+        <v>0</v>
+      </c>
+      <c r="G35" s="4">
+        <v>19</v>
+      </c>
+      <c r="H35" s="4">
+        <v>-62</v>
+      </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>11</v>
       </c>
+      <c r="B36" s="4">
+        <v>19</v>
+      </c>
+      <c r="C36" s="4">
+        <v>1</v>
+      </c>
+      <c r="D36" s="4">
+        <v>0</v>
+      </c>
+      <c r="E36" s="4">
+        <v>0</v>
+      </c>
+      <c r="F36" s="4">
+        <v>0</v>
+      </c>
+      <c r="G36" s="4">
+        <v>4</v>
+      </c>
+      <c r="H36" s="4">
+        <v>994</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>12</v>
       </c>
+      <c r="B37" s="4">
+        <v>191</v>
+      </c>
+      <c r="C37" s="4">
+        <v>1</v>
+      </c>
+      <c r="D37" s="4">
+        <v>0</v>
+      </c>
+      <c r="E37" s="4">
+        <v>0</v>
+      </c>
+      <c r="F37" s="4">
+        <v>0</v>
+      </c>
+      <c r="G37" s="4">
+        <v>36</v>
+      </c>
+      <c r="H37" s="4">
+        <v>914</v>
+      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>13</v>
       </c>
+      <c r="B38" s="4">
+        <v>491</v>
+      </c>
+      <c r="C38" s="4">
+        <v>1</v>
+      </c>
+      <c r="D38" s="4">
+        <v>6</v>
+      </c>
+      <c r="E38" s="4">
+        <v>0</v>
+      </c>
+      <c r="F38" s="4">
+        <v>0</v>
+      </c>
+      <c r="G38" s="4">
+        <v>102</v>
+      </c>
+      <c r="H38" s="4">
+        <v>844</v>
+      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>14</v>
       </c>
+      <c r="B39" s="4">
+        <v>53</v>
+      </c>
+      <c r="C39" s="4">
+        <v>1</v>
+      </c>
+      <c r="D39" s="4">
+        <v>0</v>
+      </c>
+      <c r="E39" s="4">
+        <v>0</v>
+      </c>
+      <c r="F39" s="4">
+        <v>0</v>
+      </c>
+      <c r="G39" s="4">
+        <v>10</v>
+      </c>
+      <c r="H39" s="4">
+        <v>978</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>15</v>
       </c>
+      <c r="B40" s="4">
+        <v>23</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0</v>
+      </c>
+      <c r="D40" s="4">
+        <v>0</v>
+      </c>
+      <c r="E40" s="4">
+        <v>0</v>
+      </c>
+      <c r="F40" s="4">
+        <v>0</v>
+      </c>
+      <c r="G40" s="4">
+        <v>5</v>
+      </c>
+      <c r="H40" s="4">
+        <v>-16</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>16</v>
       </c>
+      <c r="B41" s="4">
+        <v>237</v>
+      </c>
+      <c r="C41" s="4">
+        <v>0</v>
+      </c>
+      <c r="D41" s="4">
+        <v>0</v>
+      </c>
+      <c r="E41" s="4">
+        <v>0</v>
+      </c>
+      <c r="F41" s="4">
+        <v>0</v>
+      </c>
+      <c r="G41" s="4">
+        <v>45</v>
+      </c>
+      <c r="H41" s="4">
+        <v>-139</v>
+      </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>17</v>
       </c>
+      <c r="B42" s="4">
+        <v>498</v>
+      </c>
+      <c r="C42" s="4">
+        <v>1</v>
+      </c>
+      <c r="D42" s="4">
+        <v>5</v>
+      </c>
+      <c r="E42" s="4">
+        <v>0</v>
+      </c>
+      <c r="F42" s="4">
+        <v>0</v>
+      </c>
+      <c r="G42" s="4">
+        <v>103</v>
+      </c>
+      <c r="H42" s="4">
+        <v>759</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>18</v>
       </c>
+      <c r="B43" s="4">
+        <v>432</v>
+      </c>
+      <c r="C43" s="4">
+        <v>1</v>
+      </c>
+      <c r="D43" s="4">
+        <v>6</v>
+      </c>
+      <c r="E43" s="4">
+        <v>0</v>
+      </c>
+      <c r="F43" s="4">
+        <v>0</v>
+      </c>
+      <c r="G43" s="4">
+        <v>89</v>
+      </c>
+      <c r="H43" s="4">
+        <v>869</v>
+      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>19</v>
       </c>
+      <c r="B44" s="4">
+        <v>216</v>
+      </c>
+      <c r="C44" s="4">
+        <v>1</v>
+      </c>
+      <c r="D44" s="4">
+        <v>4</v>
+      </c>
+      <c r="E44" s="4">
+        <v>0</v>
+      </c>
+      <c r="F44" s="4">
+        <v>0</v>
+      </c>
+      <c r="G44" s="4">
+        <v>43</v>
+      </c>
+      <c r="H44" s="4">
+        <v>922</v>
+      </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>20</v>
       </c>
+      <c r="B45" s="4">
+        <v>112</v>
+      </c>
+      <c r="C45" s="4">
+        <v>1</v>
+      </c>
+      <c r="D45" s="4">
+        <v>0</v>
+      </c>
+      <c r="E45" s="4">
+        <v>0</v>
+      </c>
+      <c r="F45" s="4">
+        <v>0</v>
+      </c>
+      <c r="G45" s="4">
+        <v>21</v>
+      </c>
+      <c r="H45" s="4">
+        <v>939</v>
+      </c>
     </row>
     <row r="47" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
@@ -1936,117 +2359,537 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49" s="5">
+        <v>517</v>
+      </c>
+      <c r="C49" s="5">
+        <v>1</v>
+      </c>
+      <c r="D49" s="5">
+        <v>9</v>
+      </c>
+      <c r="E49" s="5">
+        <v>0</v>
+      </c>
+      <c r="F49" s="5">
+        <v>0</v>
+      </c>
+      <c r="G49" s="5">
+        <v>102</v>
+      </c>
+      <c r="H49" s="5">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B50" s="5">
+        <v>1040</v>
+      </c>
+      <c r="C50" s="5">
+        <v>1</v>
+      </c>
+      <c r="D50" s="5">
+        <v>6</v>
+      </c>
+      <c r="E50" s="5">
+        <v>0</v>
+      </c>
+      <c r="F50" s="5">
+        <v>0</v>
+      </c>
+      <c r="G50" s="5">
+        <v>217</v>
+      </c>
+      <c r="H50" s="5">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B51" s="5">
+        <v>50</v>
+      </c>
+      <c r="C51" s="5">
+        <v>0</v>
+      </c>
+      <c r="D51" s="5">
+        <v>0</v>
+      </c>
+      <c r="E51" s="5">
+        <v>0</v>
+      </c>
+      <c r="F51" s="5">
+        <v>0</v>
+      </c>
+      <c r="G51" s="5">
+        <v>10</v>
+      </c>
+      <c r="H51" s="5">
+        <v>-28</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B52" s="5">
+        <v>408</v>
+      </c>
+      <c r="C52" s="5">
+        <v>1</v>
+      </c>
+      <c r="D52" s="5">
+        <v>0</v>
+      </c>
+      <c r="E52" s="5">
+        <v>0</v>
+      </c>
+      <c r="F52" s="5">
+        <v>0</v>
+      </c>
+      <c r="G52" s="5">
+        <v>81</v>
+      </c>
+      <c r="H52" s="5">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B53" s="5">
+        <v>23</v>
+      </c>
+      <c r="C53" s="5">
+        <v>0</v>
+      </c>
+      <c r="D53" s="5">
+        <v>0</v>
+      </c>
+      <c r="E53" s="5">
+        <v>0</v>
+      </c>
+      <c r="F53" s="5">
+        <v>0</v>
+      </c>
+      <c r="G53" s="5">
+        <v>5</v>
+      </c>
+      <c r="H53" s="5">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B54" s="5">
+        <v>950</v>
+      </c>
+      <c r="C54" s="5">
+        <v>1</v>
+      </c>
+      <c r="D54" s="5">
+        <v>11</v>
+      </c>
+      <c r="E54" s="5">
+        <v>0</v>
+      </c>
+      <c r="F54" s="5">
+        <v>0</v>
+      </c>
+      <c r="G54" s="5">
+        <v>197</v>
+      </c>
+      <c r="H54" s="5">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B55" s="5">
+        <v>23</v>
+      </c>
+      <c r="C55" s="5">
+        <v>0</v>
+      </c>
+      <c r="D55" s="5">
+        <v>0</v>
+      </c>
+      <c r="E55" s="5">
+        <v>0</v>
+      </c>
+      <c r="F55" s="5">
+        <v>0</v>
+      </c>
+      <c r="G55" s="5">
+        <v>5</v>
+      </c>
+      <c r="H55" s="5">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B56" s="5">
+        <v>161</v>
+      </c>
+      <c r="C56" s="5">
+        <v>0</v>
+      </c>
+      <c r="D56" s="5">
+        <v>0</v>
+      </c>
+      <c r="E56" s="5">
+        <v>0</v>
+      </c>
+      <c r="F56" s="5">
+        <v>0</v>
+      </c>
+      <c r="G56" s="5">
+        <v>31</v>
+      </c>
+      <c r="H56" s="5">
+        <v>-92</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B57" s="5">
+        <v>587</v>
+      </c>
+      <c r="C57" s="5">
+        <v>1</v>
+      </c>
+      <c r="D57" s="5">
+        <v>7</v>
+      </c>
+      <c r="E57" s="5">
+        <v>0</v>
+      </c>
+      <c r="F57" s="5">
+        <v>0</v>
+      </c>
+      <c r="G57" s="5">
+        <v>120</v>
+      </c>
+      <c r="H57" s="5">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B58" s="5">
+        <v>169</v>
+      </c>
+      <c r="C58" s="5">
+        <v>0</v>
+      </c>
+      <c r="D58" s="5">
+        <v>0</v>
+      </c>
+      <c r="E58" s="5">
+        <v>0</v>
+      </c>
+      <c r="F58" s="5">
+        <v>0</v>
+      </c>
+      <c r="G58" s="5">
+        <v>33</v>
+      </c>
+      <c r="H58" s="5">
+        <v>-108</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B59" s="5">
+        <v>942</v>
+      </c>
+      <c r="C59" s="5">
+        <v>1</v>
+      </c>
+      <c r="D59" s="5">
+        <v>10</v>
+      </c>
+      <c r="E59" s="5">
+        <v>0</v>
+      </c>
+      <c r="F59" s="5">
+        <v>0</v>
+      </c>
+      <c r="G59" s="5">
+        <v>195</v>
+      </c>
+      <c r="H59" s="5">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B60" s="5">
+        <v>490</v>
+      </c>
+      <c r="C60" s="5">
+        <v>1</v>
+      </c>
+      <c r="D60" s="5">
+        <v>6</v>
+      </c>
+      <c r="E60" s="5">
+        <v>0</v>
+      </c>
+      <c r="F60" s="5">
+        <v>0</v>
+      </c>
+      <c r="G60" s="5">
+        <v>99</v>
+      </c>
+      <c r="H60" s="5">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B61" s="5">
+        <v>118</v>
+      </c>
+      <c r="C61" s="5">
+        <v>1</v>
+      </c>
+      <c r="D61" s="5">
+        <v>0</v>
+      </c>
+      <c r="E61" s="5">
+        <v>0</v>
+      </c>
+      <c r="F61" s="5">
+        <v>0</v>
+      </c>
+      <c r="G61" s="5">
+        <v>23</v>
+      </c>
+      <c r="H61" s="5">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B62" s="5">
+        <v>955</v>
+      </c>
+      <c r="C62" s="5">
+        <v>1</v>
+      </c>
+      <c r="D62" s="5">
+        <v>0</v>
+      </c>
+      <c r="E62" s="5">
+        <v>0</v>
+      </c>
+      <c r="F62" s="5">
+        <v>0</v>
+      </c>
+      <c r="G62" s="5">
+        <v>196</v>
+      </c>
+      <c r="H62" s="5">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B63" s="5">
+        <v>598</v>
+      </c>
+      <c r="C63" s="5">
+        <v>1</v>
+      </c>
+      <c r="D63" s="5">
+        <v>0</v>
+      </c>
+      <c r="E63" s="5">
+        <v>0</v>
+      </c>
+      <c r="F63" s="5">
+        <v>0</v>
+      </c>
+      <c r="G63" s="5">
+        <v>119</v>
+      </c>
+      <c r="H63" s="5">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>16</v>
+      </c>
+      <c r="B64" s="5">
+        <v>73</v>
+      </c>
+      <c r="C64" s="5">
+        <v>0</v>
+      </c>
+      <c r="D64" s="5">
+        <v>0</v>
+      </c>
+      <c r="E64" s="5">
+        <v>0</v>
+      </c>
+      <c r="F64" s="5">
+        <v>0</v>
+      </c>
+      <c r="G64" s="5">
+        <v>13</v>
+      </c>
+      <c r="H64" s="5">
+        <v>-36</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>17</v>
       </c>
+      <c r="B65" s="5">
+        <v>495</v>
+      </c>
+      <c r="C65" s="5">
+        <v>1</v>
+      </c>
+      <c r="D65" s="5">
+        <v>5</v>
+      </c>
+      <c r="E65" s="5">
+        <v>0</v>
+      </c>
+      <c r="F65" s="5">
+        <v>0</v>
+      </c>
+      <c r="G65" s="5">
+        <v>98</v>
+      </c>
+      <c r="H65" s="5">
+        <v>847</v>
+      </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>18</v>
       </c>
+      <c r="B66" s="5">
+        <v>331</v>
+      </c>
+      <c r="C66" s="5">
+        <v>1</v>
+      </c>
+      <c r="D66" s="5">
+        <v>0</v>
+      </c>
+      <c r="E66" s="5">
+        <v>0</v>
+      </c>
+      <c r="F66" s="5">
+        <v>0</v>
+      </c>
+      <c r="G66" s="5">
+        <v>64</v>
+      </c>
+      <c r="H66" s="5">
+        <v>835</v>
+      </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>19</v>
       </c>
+      <c r="B67" s="5">
+        <v>23</v>
+      </c>
+      <c r="C67" s="5">
+        <v>0</v>
+      </c>
+      <c r="D67" s="5">
+        <v>0</v>
+      </c>
+      <c r="E67" s="5">
+        <v>0</v>
+      </c>
+      <c r="F67" s="5">
+        <v>0</v>
+      </c>
+      <c r="G67" s="5">
+        <v>5</v>
+      </c>
+      <c r="H67" s="5">
+        <v>-16</v>
+      </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>20</v>
       </c>
+      <c r="B68" s="5">
+        <v>58</v>
+      </c>
+      <c r="C68" s="5">
+        <v>0</v>
+      </c>
+      <c r="D68" s="5">
+        <v>0</v>
+      </c>
+      <c r="E68" s="5">
+        <v>0</v>
+      </c>
+      <c r="F68" s="5">
+        <v>0</v>
+      </c>
+      <c r="G68" s="5">
+        <v>10</v>
+      </c>
+      <c r="H68" s="5">
+        <v>-26</v>
+      </c>
     </row>
     <row r="70" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A70" s="8" t="s">
+      <c r="A70" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B70" s="8"/>
-      <c r="C70" s="8"/>
-      <c r="D70" s="8"/>
-      <c r="E70" s="8"/>
-      <c r="F70" s="8"/>
-      <c r="G70" s="8"/>
-      <c r="H70" s="8"/>
+      <c r="B70" s="9"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="9"/>
+      <c r="H70" s="9"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
@@ -2077,114 +2920,534 @@
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>1</v>
+      </c>
+      <c r="B72" s="5">
+        <v>1674</v>
+      </c>
+      <c r="C72" s="5">
+        <v>1</v>
+      </c>
+      <c r="D72" s="5">
+        <v>12</v>
+      </c>
+      <c r="E72" s="5">
+        <v>0</v>
+      </c>
+      <c r="F72" s="5">
+        <v>0</v>
+      </c>
+      <c r="G72" s="5">
+        <v>343</v>
+      </c>
+      <c r="H72" s="5">
+        <v>467</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>2</v>
       </c>
+      <c r="B73" s="5">
+        <v>968</v>
+      </c>
+      <c r="C73" s="5">
+        <v>1</v>
+      </c>
+      <c r="D73" s="5">
+        <v>16</v>
+      </c>
+      <c r="E73" s="5">
+        <v>0</v>
+      </c>
+      <c r="F73" s="5">
+        <v>0</v>
+      </c>
+      <c r="G73" s="5">
+        <v>195</v>
+      </c>
+      <c r="H73" s="5">
+        <v>857</v>
+      </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>3</v>
       </c>
+      <c r="B74" s="5">
+        <v>865</v>
+      </c>
+      <c r="C74" s="5">
+        <v>1</v>
+      </c>
+      <c r="D74" s="5">
+        <v>10</v>
+      </c>
+      <c r="E74" s="5">
+        <v>0</v>
+      </c>
+      <c r="F74" s="5">
+        <v>0</v>
+      </c>
+      <c r="G74" s="5">
+        <v>176</v>
+      </c>
+      <c r="H74" s="5">
+        <v>674</v>
+      </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>4</v>
       </c>
+      <c r="B75" s="5">
+        <v>746</v>
+      </c>
+      <c r="C75" s="5">
+        <v>1</v>
+      </c>
+      <c r="D75" s="5">
+        <v>0</v>
+      </c>
+      <c r="E75" s="5">
+        <v>0</v>
+      </c>
+      <c r="F75" s="5">
+        <v>0</v>
+      </c>
+      <c r="G75" s="5">
+        <v>151</v>
+      </c>
+      <c r="H75" s="5">
+        <v>658</v>
+      </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>5</v>
       </c>
+      <c r="B76" s="5">
+        <v>80</v>
+      </c>
+      <c r="C76" s="5">
+        <v>0</v>
+      </c>
+      <c r="D76" s="5">
+        <v>0</v>
+      </c>
+      <c r="E76" s="5">
+        <v>0</v>
+      </c>
+      <c r="F76" s="5">
+        <v>0</v>
+      </c>
+      <c r="G76" s="5">
+        <v>16</v>
+      </c>
+      <c r="H76" s="5">
+        <v>-57</v>
+      </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>6</v>
       </c>
+      <c r="B77" s="5">
+        <v>919</v>
+      </c>
+      <c r="C77" s="5">
+        <v>1</v>
+      </c>
+      <c r="D77" s="5">
+        <v>15</v>
+      </c>
+      <c r="E77" s="5">
+        <v>0</v>
+      </c>
+      <c r="F77" s="5">
+        <v>0</v>
+      </c>
+      <c r="G77" s="5">
+        <v>188</v>
+      </c>
+      <c r="H77" s="5">
+        <v>796</v>
+      </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>7</v>
       </c>
+      <c r="B78" s="5">
+        <v>158</v>
+      </c>
+      <c r="C78" s="5">
+        <v>0</v>
+      </c>
+      <c r="D78" s="5">
+        <v>0</v>
+      </c>
+      <c r="E78" s="5">
+        <v>0</v>
+      </c>
+      <c r="F78" s="5">
+        <v>0</v>
+      </c>
+      <c r="G78" s="5">
+        <v>30</v>
+      </c>
+      <c r="H78" s="5">
+        <v>-95</v>
+      </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>8</v>
       </c>
+      <c r="B79" s="5">
+        <v>44</v>
+      </c>
+      <c r="C79" s="5">
+        <v>0</v>
+      </c>
+      <c r="D79" s="5">
+        <v>0</v>
+      </c>
+      <c r="E79" s="5">
+        <v>0</v>
+      </c>
+      <c r="F79" s="5">
+        <v>0</v>
+      </c>
+      <c r="G79" s="5">
+        <v>8</v>
+      </c>
+      <c r="H79" s="5">
+        <v>-25</v>
+      </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>9</v>
       </c>
+      <c r="B80" s="5">
+        <v>293</v>
+      </c>
+      <c r="C80" s="5">
+        <v>1</v>
+      </c>
+      <c r="D80" s="5">
+        <v>0</v>
+      </c>
+      <c r="E80" s="5">
+        <v>0</v>
+      </c>
+      <c r="F80" s="5">
+        <v>0</v>
+      </c>
+      <c r="G80" s="5">
+        <v>58</v>
+      </c>
+      <c r="H80" s="5">
+        <v>886</v>
+      </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>10</v>
       </c>
+      <c r="B81" s="5">
+        <v>63</v>
+      </c>
+      <c r="C81" s="5">
+        <v>0</v>
+      </c>
+      <c r="D81" s="5">
+        <v>0</v>
+      </c>
+      <c r="E81" s="5">
+        <v>0</v>
+      </c>
+      <c r="F81" s="5">
+        <v>0</v>
+      </c>
+      <c r="G81" s="5">
+        <v>11</v>
+      </c>
+      <c r="H81" s="5">
+        <v>-28</v>
+      </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>11</v>
       </c>
+      <c r="B82" s="5">
+        <v>23</v>
+      </c>
+      <c r="C82" s="5">
+        <v>0</v>
+      </c>
+      <c r="D82" s="5">
+        <v>0</v>
+      </c>
+      <c r="E82" s="5">
+        <v>0</v>
+      </c>
+      <c r="F82" s="5">
+        <v>0</v>
+      </c>
+      <c r="G82" s="5">
+        <v>5</v>
+      </c>
+      <c r="H82" s="5">
+        <v>-16</v>
+      </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>12</v>
       </c>
+      <c r="B83" s="5">
+        <v>116</v>
+      </c>
+      <c r="C83" s="5">
+        <v>0</v>
+      </c>
+      <c r="D83" s="5">
+        <v>0</v>
+      </c>
+      <c r="E83" s="5">
+        <v>0</v>
+      </c>
+      <c r="F83" s="5">
+        <v>0</v>
+      </c>
+      <c r="G83" s="5">
+        <v>22</v>
+      </c>
+      <c r="H83" s="5">
+        <v>-72</v>
+      </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>13</v>
       </c>
+      <c r="B84" s="5">
+        <v>1759</v>
+      </c>
+      <c r="C84" s="5">
+        <v>1</v>
+      </c>
+      <c r="D84" s="5">
+        <v>13</v>
+      </c>
+      <c r="E84" s="5">
+        <v>0</v>
+      </c>
+      <c r="F84" s="5">
+        <v>0</v>
+      </c>
+      <c r="G84" s="5">
+        <v>354</v>
+      </c>
+      <c r="H84" s="5">
+        <v>371</v>
+      </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>14</v>
       </c>
+      <c r="B85" s="5">
+        <v>552</v>
+      </c>
+      <c r="C85" s="5">
+        <v>1</v>
+      </c>
+      <c r="D85" s="5">
+        <v>0</v>
+      </c>
+      <c r="E85" s="5">
+        <v>0</v>
+      </c>
+      <c r="F85" s="5">
+        <v>0</v>
+      </c>
+      <c r="G85" s="5">
+        <v>113</v>
+      </c>
+      <c r="H85" s="5">
+        <v>701</v>
+      </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>15</v>
       </c>
+      <c r="B86" s="5">
+        <v>23</v>
+      </c>
+      <c r="C86" s="5">
+        <v>0</v>
+      </c>
+      <c r="D86" s="5">
+        <v>0</v>
+      </c>
+      <c r="E86" s="5">
+        <v>0</v>
+      </c>
+      <c r="F86" s="5">
+        <v>0</v>
+      </c>
+      <c r="G86" s="5">
+        <v>5</v>
+      </c>
+      <c r="H86" s="5">
+        <v>-16</v>
+      </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>16</v>
       </c>
+      <c r="B87" s="5">
+        <v>214</v>
+      </c>
+      <c r="C87" s="5">
+        <v>1</v>
+      </c>
+      <c r="D87" s="5">
+        <v>0</v>
+      </c>
+      <c r="E87" s="5">
+        <v>0</v>
+      </c>
+      <c r="F87" s="5">
+        <v>0</v>
+      </c>
+      <c r="G87" s="5">
+        <v>45</v>
+      </c>
+      <c r="H87" s="5">
+        <v>925</v>
+      </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>17</v>
       </c>
+      <c r="B88" s="5">
+        <v>221</v>
+      </c>
+      <c r="C88" s="5">
+        <v>0</v>
+      </c>
+      <c r="D88" s="5">
+        <v>0</v>
+      </c>
+      <c r="E88" s="5">
+        <v>0</v>
+      </c>
+      <c r="F88" s="5">
+        <v>0</v>
+      </c>
+      <c r="G88" s="5">
+        <v>43</v>
+      </c>
+      <c r="H88" s="5">
+        <v>-144</v>
+      </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>18</v>
       </c>
+      <c r="B89" s="5">
+        <v>64</v>
+      </c>
+      <c r="C89" s="5">
+        <v>0</v>
+      </c>
+      <c r="D89" s="5">
+        <v>0</v>
+      </c>
+      <c r="E89" s="5">
+        <v>0</v>
+      </c>
+      <c r="F89" s="5">
+        <v>0</v>
+      </c>
+      <c r="G89" s="5">
+        <v>12</v>
+      </c>
+      <c r="H89" s="5">
+        <v>-31</v>
+      </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>19</v>
       </c>
+      <c r="B90" s="5">
+        <v>308</v>
+      </c>
+      <c r="C90" s="5">
+        <v>1</v>
+      </c>
+      <c r="D90" s="5">
+        <v>0</v>
+      </c>
+      <c r="E90" s="5">
+        <v>0</v>
+      </c>
+      <c r="F90" s="5">
+        <v>0</v>
+      </c>
+      <c r="G90" s="5">
+        <v>63</v>
+      </c>
+      <c r="H90" s="5">
+        <v>898</v>
+      </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>20</v>
       </c>
+      <c r="B91" s="5">
+        <v>1137</v>
+      </c>
+      <c r="C91" s="5">
+        <v>1</v>
+      </c>
+      <c r="D91" s="5">
+        <v>16</v>
+      </c>
+      <c r="E91" s="5">
+        <v>0</v>
+      </c>
+      <c r="F91" s="5">
+        <v>0</v>
+      </c>
+      <c r="G91" s="5">
+        <v>232</v>
+      </c>
+      <c r="H91" s="5">
+        <v>825</v>
+      </c>
     </row>
     <row r="93" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A93" s="8" t="s">
+      <c r="A93" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B93" s="8"/>
-      <c r="C93" s="8"/>
-      <c r="D93" s="8"/>
-      <c r="E93" s="8"/>
-      <c r="F93" s="8"/>
-      <c r="G93" s="8"/>
-      <c r="H93" s="8"/>
+      <c r="B93" s="9"/>
+      <c r="C93" s="9"/>
+      <c r="D93" s="9"/>
+      <c r="E93" s="9"/>
+      <c r="F93" s="9"/>
+      <c r="G93" s="9"/>
+      <c r="H93" s="9"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
@@ -2215,101 +3478,521 @@
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>1</v>
+      </c>
+      <c r="B95" s="5">
+        <v>1033</v>
+      </c>
+      <c r="C95" s="5">
+        <v>1</v>
+      </c>
+      <c r="D95" s="5">
+        <v>17</v>
+      </c>
+      <c r="E95" s="5">
+        <v>0</v>
+      </c>
+      <c r="F95" s="5">
+        <v>0</v>
+      </c>
+      <c r="G95" s="5">
+        <v>210</v>
+      </c>
+      <c r="H95" s="5">
+        <v>772</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B96" s="5">
+        <v>862</v>
+      </c>
+      <c r="C96" s="5">
+        <v>1</v>
+      </c>
+      <c r="D96" s="5">
+        <v>19</v>
+      </c>
+      <c r="E96" s="5">
+        <v>0</v>
+      </c>
+      <c r="F96" s="5">
+        <v>0</v>
+      </c>
+      <c r="G96" s="5">
+        <v>175</v>
+      </c>
+      <c r="H96" s="5">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B97" s="5">
+        <v>2214</v>
+      </c>
+      <c r="C97" s="5">
+        <v>1</v>
+      </c>
+      <c r="D97" s="5">
+        <v>14</v>
+      </c>
+      <c r="E97" s="5">
+        <v>0</v>
+      </c>
+      <c r="F97" s="5">
+        <v>0</v>
+      </c>
+      <c r="G97" s="5">
+        <v>453</v>
+      </c>
+      <c r="H97" s="5">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B98" s="5">
+        <v>712</v>
+      </c>
+      <c r="C98" s="5">
+        <v>1</v>
+      </c>
+      <c r="D98" s="5">
+        <v>20</v>
+      </c>
+      <c r="E98" s="5">
+        <v>0</v>
+      </c>
+      <c r="F98" s="5">
+        <v>0</v>
+      </c>
+      <c r="G98" s="5">
+        <v>145</v>
+      </c>
+      <c r="H98" s="5">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B99" s="5">
+        <v>689</v>
+      </c>
+      <c r="C99" s="5">
+        <v>1</v>
+      </c>
+      <c r="D99" s="5">
+        <v>14</v>
+      </c>
+      <c r="E99" s="5">
+        <v>0</v>
+      </c>
+      <c r="F99" s="5">
+        <v>0</v>
+      </c>
+      <c r="G99" s="5">
+        <v>140</v>
+      </c>
+      <c r="H99" s="5">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B100" s="5">
+        <v>522</v>
+      </c>
+      <c r="C100" s="5">
+        <v>1</v>
+      </c>
+      <c r="D100" s="5">
+        <v>0</v>
+      </c>
+      <c r="E100" s="5">
+        <v>0</v>
+      </c>
+      <c r="F100" s="5">
+        <v>0</v>
+      </c>
+      <c r="G100" s="5">
+        <v>103</v>
+      </c>
+      <c r="H100" s="5">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B101" s="5">
+        <v>1558</v>
+      </c>
+      <c r="C101" s="5">
+        <v>1</v>
+      </c>
+      <c r="D101" s="5">
+        <v>21</v>
+      </c>
+      <c r="E101" s="5">
+        <v>0</v>
+      </c>
+      <c r="F101" s="5">
+        <v>0</v>
+      </c>
+      <c r="G101" s="5">
+        <v>315</v>
+      </c>
+      <c r="H101" s="5">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B102" s="5">
+        <v>62</v>
+      </c>
+      <c r="C102" s="5">
+        <v>0</v>
+      </c>
+      <c r="D102" s="5">
+        <v>0</v>
+      </c>
+      <c r="E102" s="5">
+        <v>0</v>
+      </c>
+      <c r="F102" s="5">
+        <v>0</v>
+      </c>
+      <c r="G102" s="5">
+        <v>12</v>
+      </c>
+      <c r="H102" s="5">
+        <v>-36</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B103" s="5">
+        <v>48</v>
+      </c>
+      <c r="C103" s="5">
+        <v>0</v>
+      </c>
+      <c r="D103" s="5">
+        <v>0</v>
+      </c>
+      <c r="E103" s="5">
+        <v>0</v>
+      </c>
+      <c r="F103" s="5">
+        <v>0</v>
+      </c>
+      <c r="G103" s="5">
+        <v>10</v>
+      </c>
+      <c r="H103" s="5">
+        <v>-32</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B104" s="5">
+        <v>1068</v>
+      </c>
+      <c r="C104" s="5">
+        <v>1</v>
+      </c>
+      <c r="D104" s="5">
+        <v>0</v>
+      </c>
+      <c r="E104" s="5">
+        <v>0</v>
+      </c>
+      <c r="F104" s="5">
+        <v>0</v>
+      </c>
+      <c r="G104" s="5">
+        <v>213</v>
+      </c>
+      <c r="H104" s="5">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B105" s="5">
+        <v>1662</v>
+      </c>
+      <c r="C105" s="5">
+        <v>1</v>
+      </c>
+      <c r="D105" s="5">
+        <v>0</v>
+      </c>
+      <c r="E105" s="5">
+        <v>0</v>
+      </c>
+      <c r="F105" s="5">
+        <v>0</v>
+      </c>
+      <c r="G105" s="5">
+        <v>339</v>
+      </c>
+      <c r="H105" s="5">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B106" s="5">
+        <v>931</v>
+      </c>
+      <c r="C106" s="5">
+        <v>1</v>
+      </c>
+      <c r="D106" s="5">
+        <v>0</v>
+      </c>
+      <c r="E106" s="5">
+        <v>0</v>
+      </c>
+      <c r="F106" s="5">
+        <v>0</v>
+      </c>
+      <c r="G106" s="5">
+        <v>190</v>
+      </c>
+      <c r="H106" s="5">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B107" s="5">
+        <v>275</v>
+      </c>
+      <c r="C107" s="5">
+        <v>1</v>
+      </c>
+      <c r="D107" s="5">
+        <v>0</v>
+      </c>
+      <c r="E107" s="5">
+        <v>0</v>
+      </c>
+      <c r="F107" s="5">
+        <v>0</v>
+      </c>
+      <c r="G107" s="5">
+        <v>56</v>
+      </c>
+      <c r="H107" s="5">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B108" s="5">
+        <v>2187</v>
+      </c>
+      <c r="C108" s="5">
+        <v>1</v>
+      </c>
+      <c r="D108" s="5">
+        <v>19</v>
+      </c>
+      <c r="E108" s="5">
+        <v>0</v>
+      </c>
+      <c r="F108" s="5">
+        <v>0</v>
+      </c>
+      <c r="G108" s="5">
+        <v>448</v>
+      </c>
+      <c r="H108" s="5">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B109" s="5">
+        <v>1192</v>
+      </c>
+      <c r="C109" s="5">
+        <v>1</v>
+      </c>
+      <c r="D109" s="5">
+        <v>0</v>
+      </c>
+      <c r="E109" s="5">
+        <v>0</v>
+      </c>
+      <c r="F109" s="5">
+        <v>0</v>
+      </c>
+      <c r="G109" s="5">
+        <v>241</v>
+      </c>
+      <c r="H109" s="5">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B110" s="5">
+        <v>1745</v>
+      </c>
+      <c r="C110" s="5">
+        <v>1</v>
+      </c>
+      <c r="D110" s="5">
+        <v>19</v>
+      </c>
+      <c r="E110" s="5">
+        <v>0</v>
+      </c>
+      <c r="F110" s="5">
+        <v>0</v>
+      </c>
+      <c r="G110" s="5">
+        <v>356</v>
+      </c>
+      <c r="H110" s="5">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B111" s="5">
+        <v>131</v>
+      </c>
+      <c r="C111" s="5">
+        <v>0</v>
+      </c>
+      <c r="D111" s="5">
+        <v>0</v>
+      </c>
+      <c r="E111" s="5">
+        <v>0</v>
+      </c>
+      <c r="F111" s="5">
+        <v>0</v>
+      </c>
+      <c r="G111" s="5">
+        <v>25</v>
+      </c>
+      <c r="H111" s="5">
+        <v>-70</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B112" s="5">
+        <v>39</v>
+      </c>
+      <c r="C112" s="5">
+        <v>0</v>
+      </c>
+      <c r="D112" s="5">
+        <v>0</v>
+      </c>
+      <c r="E112" s="5">
+        <v>0</v>
+      </c>
+      <c r="F112" s="5">
+        <v>0</v>
+      </c>
+      <c r="G112" s="5">
+        <v>7</v>
+      </c>
+      <c r="H112" s="5">
+        <v>-19</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B113" s="5">
+        <v>2208</v>
+      </c>
+      <c r="C113" s="5">
+        <v>1</v>
+      </c>
+      <c r="D113" s="5">
+        <v>20</v>
+      </c>
+      <c r="E113" s="5">
+        <v>0</v>
+      </c>
+      <c r="F113" s="5">
+        <v>0</v>
+      </c>
+      <c r="G113" s="5">
+        <v>455</v>
+      </c>
+      <c r="H113" s="5">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>20</v>
+      </c>
+      <c r="B114" s="5">
+        <v>439</v>
+      </c>
+      <c r="C114" s="5">
+        <v>1</v>
+      </c>
+      <c r="D114" s="5">
+        <v>19</v>
+      </c>
+      <c r="E114" s="5">
+        <v>0</v>
+      </c>
+      <c r="F114" s="5">
+        <v>0</v>
+      </c>
+      <c r="G114" s="5">
+        <v>88</v>
+      </c>
+      <c r="H114" s="5">
+        <v>1073</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor fix to static decisions_made varaible
</commit_message>
<xml_diff>
--- a/CSCI446_Project2_WumpusWorld/references/statistics/AgentRunStatistics.xlsx
+++ b/CSCI446_Project2_WumpusWorld/references/statistics/AgentRunStatistics.xlsx
@@ -1189,8 +1189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,10 +1248,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <v>67</v>
+        <v>21411</v>
       </c>
       <c r="C3" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="4">
         <v>0</v>
@@ -1263,10 +1263,10 @@
         <v>0</v>
       </c>
       <c r="G3" s="4">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H3" s="4">
-        <v>973</v>
+        <v>-54</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1274,10 +1274,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="4">
-        <v>108</v>
+        <v>146</v>
       </c>
       <c r="C4" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="4">
         <v>0</v>
@@ -1289,10 +1289,10 @@
         <v>0</v>
       </c>
       <c r="G4" s="4">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="H4" s="4">
-        <v>951</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1300,7 +1300,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>23</v>
+        <v>768</v>
       </c>
       <c r="C5" s="4">
         <v>0</v>
@@ -1315,10 +1315,10 @@
         <v>0</v>
       </c>
       <c r="G5" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H5" s="4">
-        <v>-16</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1326,7 +1326,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4">
-        <v>34</v>
+        <v>1617</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
@@ -1344,7 +1344,7 @@
         <v>7</v>
       </c>
       <c r="H6" s="4">
-        <v>980</v>
+        <v>989</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1352,13 +1352,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="4">
-        <v>115</v>
+        <v>18292</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
       </c>
       <c r="D7" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="4">
         <v>0</v>
@@ -1367,10 +1367,10 @@
         <v>0</v>
       </c>
       <c r="G7" s="4">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H7" s="4">
-        <v>957</v>
+        <v>954</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1378,13 +1378,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="4">
-        <v>112</v>
+        <v>10131</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
       </c>
       <c r="D8" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E8" s="4">
         <v>0</v>
@@ -1393,10 +1393,10 @@
         <v>0</v>
       </c>
       <c r="G8" s="4">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="H8" s="4">
-        <v>967</v>
+        <v>976</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1404,10 +1404,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="4">
-        <v>49</v>
+        <v>768</v>
       </c>
       <c r="C9" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="4">
         <v>0</v>
@@ -1419,10 +1419,10 @@
         <v>0</v>
       </c>
       <c r="G9" s="4">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H9" s="4">
-        <v>967</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1430,7 +1430,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="4">
-        <v>63</v>
+        <v>17114</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
@@ -1445,10 +1445,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="4">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H10" s="4">
-        <v>974</v>
+        <v>960</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1456,13 +1456,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="4">
-        <v>44</v>
+        <v>10871</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
       </c>
       <c r="D11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="4">
         <v>0</v>
@@ -1471,10 +1471,10 @@
         <v>0</v>
       </c>
       <c r="G11" s="4">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="H11" s="4">
-        <v>976</v>
+        <v>954</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1482,10 +1482,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="4">
-        <v>33</v>
+        <v>6529</v>
       </c>
       <c r="C12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="4">
         <v>0</v>
@@ -1497,10 +1497,10 @@
         <v>0</v>
       </c>
       <c r="G12" s="4">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="H12" s="4">
-        <v>-24</v>
+        <v>968</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1508,13 +1508,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="4">
-        <v>10</v>
+        <v>2301</v>
       </c>
       <c r="C13" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E13" s="4">
         <v>0</v>
@@ -1523,10 +1523,10 @@
         <v>0</v>
       </c>
       <c r="G13" s="4">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="H13" s="4">
-        <v>-7</v>
+        <v>991</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1534,13 +1534,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="4">
-        <v>123</v>
+        <v>8342</v>
       </c>
       <c r="C14" s="4">
         <v>1</v>
       </c>
       <c r="D14" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="4">
         <v>0</v>
@@ -1549,10 +1549,10 @@
         <v>0</v>
       </c>
       <c r="G14" s="4">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="H14" s="4">
-        <v>958</v>
+        <v>970</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1560,7 +1560,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="4">
-        <v>98</v>
+        <v>5832</v>
       </c>
       <c r="C15" s="4">
         <v>1</v>
@@ -1575,10 +1575,10 @@
         <v>0</v>
       </c>
       <c r="G15" s="4">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="H15" s="4">
-        <v>962</v>
+        <v>977</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1586,7 +1586,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="4">
-        <v>92</v>
+        <v>146</v>
       </c>
       <c r="C16" s="4">
         <v>0</v>
@@ -1601,10 +1601,10 @@
         <v>0</v>
       </c>
       <c r="G16" s="4">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="H16" s="4">
-        <v>-44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1612,10 +1612,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="4">
-        <v>48</v>
+        <v>24083</v>
       </c>
       <c r="C17" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="4">
         <v>0</v>
@@ -1627,10 +1627,10 @@
         <v>0</v>
       </c>
       <c r="G17" s="4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H17" s="4">
-        <v>-26</v>
+        <v>944</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1638,7 +1638,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="4">
-        <v>64</v>
+        <v>9426</v>
       </c>
       <c r="C18" s="4">
         <v>1</v>
@@ -1653,10 +1653,10 @@
         <v>0</v>
       </c>
       <c r="G18" s="4">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H18" s="4">
-        <v>976</v>
+        <v>958</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1664,10 +1664,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="4">
-        <v>10</v>
+        <v>15410</v>
       </c>
       <c r="C19" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="4">
         <v>0</v>
@@ -1679,10 +1679,10 @@
         <v>0</v>
       </c>
       <c r="G19" s="4">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="H19" s="4">
-        <v>-7</v>
+        <v>953</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1690,10 +1690,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="4">
-        <v>55</v>
+        <v>4716</v>
       </c>
       <c r="C20" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="4">
         <v>0</v>
@@ -1705,10 +1705,10 @@
         <v>0</v>
       </c>
       <c r="G20" s="4">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H20" s="4">
-        <v>-36</v>
+        <v>980</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1716,13 +1716,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="4">
-        <v>48</v>
+        <v>8061</v>
       </c>
       <c r="C21" s="4">
         <v>1</v>
       </c>
       <c r="D21" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="4">
         <v>0</v>
@@ -1731,10 +1731,10 @@
         <v>0</v>
       </c>
       <c r="G21" s="4">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H21" s="4">
-        <v>978</v>
+        <v>957</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1742,13 +1742,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="4">
-        <v>104</v>
+        <v>5430</v>
       </c>
       <c r="C22" s="4">
         <v>1</v>
       </c>
       <c r="D22" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" s="4">
         <v>0</v>
@@ -1757,10 +1757,10 @@
         <v>0</v>
       </c>
       <c r="G22" s="4">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="H22" s="4">
-        <v>967</v>
+        <v>981</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Redid all runs with new decisions made appraoch
</commit_message>
<xml_diff>
--- a/CSCI446_Project2_WumpusWorld/references/statistics/AgentRunStatistics.xlsx
+++ b/CSCI446_Project2_WumpusWorld/references/statistics/AgentRunStatistics.xlsx
@@ -1189,8 +1189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="J107" sqref="J107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1806,10 +1806,10 @@
         <v>1</v>
       </c>
       <c r="B26" s="4">
-        <v>50</v>
+        <v>13870</v>
       </c>
       <c r="C26" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" s="4">
         <v>0</v>
@@ -1821,10 +1821,10 @@
         <v>0</v>
       </c>
       <c r="G26" s="4">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="H26" s="4">
-        <v>-28</v>
+        <v>961</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1832,10 +1832,10 @@
         <v>2</v>
       </c>
       <c r="B27" s="4">
-        <v>69</v>
+        <v>30041</v>
       </c>
       <c r="C27" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" s="4">
         <v>0</v>
@@ -1847,10 +1847,10 @@
         <v>0</v>
       </c>
       <c r="G27" s="4">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="H27" s="4">
-        <v>-40</v>
+        <v>938</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1858,10 +1858,10 @@
         <v>3</v>
       </c>
       <c r="B28" s="4">
-        <v>78</v>
+        <v>17121</v>
       </c>
       <c r="C28" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28" s="4">
         <v>0</v>
@@ -1873,10 +1873,10 @@
         <v>0</v>
       </c>
       <c r="G28" s="4">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H28" s="4">
-        <v>969</v>
+        <v>-32</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1884,13 +1884,13 @@
         <v>4</v>
       </c>
       <c r="B29" s="4">
-        <v>19</v>
+        <v>98899</v>
       </c>
       <c r="C29" s="4">
         <v>1</v>
       </c>
       <c r="D29" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E29" s="4">
         <v>0</v>
@@ -1899,10 +1899,10 @@
         <v>0</v>
       </c>
       <c r="G29" s="4">
-        <v>4</v>
+        <v>98</v>
       </c>
       <c r="H29" s="4">
-        <v>994</v>
+        <v>797</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1910,13 +1910,13 @@
         <v>5</v>
       </c>
       <c r="B30" s="4">
-        <v>139</v>
+        <v>74683</v>
       </c>
       <c r="C30" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E30" s="4">
         <v>0</v>
@@ -1925,10 +1925,10 @@
         <v>0</v>
       </c>
       <c r="G30" s="4">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="H30" s="4">
-        <v>-90</v>
+        <v>853</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1936,13 +1936,13 @@
         <v>6</v>
       </c>
       <c r="B31" s="4">
-        <v>471</v>
+        <v>6110</v>
       </c>
       <c r="C31" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E31" s="4">
         <v>0</v>
@@ -1951,10 +1951,10 @@
         <v>0</v>
       </c>
       <c r="G31" s="4">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="H31" s="4">
-        <v>817</v>
+        <v>-16</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1962,13 +1962,13 @@
         <v>7</v>
       </c>
       <c r="B32" s="4">
-        <v>408</v>
+        <v>88583</v>
       </c>
       <c r="C32" s="4">
         <v>1</v>
       </c>
       <c r="D32" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E32" s="4">
         <v>0</v>
@@ -1977,10 +1977,10 @@
         <v>0</v>
       </c>
       <c r="G32" s="4">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="H32" s="4">
-        <v>849</v>
+        <v>912</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1988,13 +1988,13 @@
         <v>8</v>
       </c>
       <c r="B33" s="4">
-        <v>23</v>
+        <v>98820</v>
       </c>
       <c r="C33" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E33" s="4">
         <v>0</v>
@@ -2003,10 +2003,10 @@
         <v>0</v>
       </c>
       <c r="G33" s="4">
-        <v>5</v>
+        <v>101</v>
       </c>
       <c r="H33" s="4">
-        <v>-16</v>
+        <v>785</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2014,7 +2014,7 @@
         <v>9</v>
       </c>
       <c r="B34" s="4">
-        <v>43</v>
+        <v>67218</v>
       </c>
       <c r="C34" s="4">
         <v>1</v>
@@ -2029,10 +2029,10 @@
         <v>0</v>
       </c>
       <c r="G34" s="4">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="H34" s="4">
-        <v>982</v>
+        <v>838</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2040,7 +2040,7 @@
         <v>10</v>
       </c>
       <c r="B35" s="4">
-        <v>101</v>
+        <v>17052</v>
       </c>
       <c r="C35" s="4">
         <v>0</v>
@@ -2055,10 +2055,10 @@
         <v>0</v>
       </c>
       <c r="G35" s="4">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="H35" s="4">
-        <v>-62</v>
+        <v>-28</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2066,13 +2066,13 @@
         <v>11</v>
       </c>
       <c r="B36" s="4">
-        <v>19</v>
+        <v>109761</v>
       </c>
       <c r="C36" s="4">
         <v>1</v>
       </c>
       <c r="D36" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E36" s="4">
         <v>0</v>
@@ -2081,10 +2081,10 @@
         <v>0</v>
       </c>
       <c r="G36" s="4">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="H36" s="4">
-        <v>994</v>
+        <v>901</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -2092,13 +2092,13 @@
         <v>12</v>
       </c>
       <c r="B37" s="4">
-        <v>191</v>
+        <v>109075</v>
       </c>
       <c r="C37" s="4">
         <v>1</v>
       </c>
       <c r="D37" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E37" s="4">
         <v>0</v>
@@ -2107,10 +2107,10 @@
         <v>0</v>
       </c>
       <c r="G37" s="4">
-        <v>36</v>
+        <v>94</v>
       </c>
       <c r="H37" s="4">
-        <v>914</v>
+        <v>861</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2118,13 +2118,13 @@
         <v>13</v>
       </c>
       <c r="B38" s="4">
-        <v>491</v>
+        <v>33121</v>
       </c>
       <c r="C38" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E38" s="4">
         <v>0</v>
@@ -2133,10 +2133,10 @@
         <v>0</v>
       </c>
       <c r="G38" s="4">
-        <v>102</v>
+        <v>18</v>
       </c>
       <c r="H38" s="4">
-        <v>844</v>
+        <v>-51</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -2144,7 +2144,7 @@
         <v>14</v>
       </c>
       <c r="B39" s="4">
-        <v>53</v>
+        <v>109560</v>
       </c>
       <c r="C39" s="4">
         <v>1</v>
@@ -2159,10 +2159,10 @@
         <v>0</v>
       </c>
       <c r="G39" s="4">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="H39" s="4">
-        <v>978</v>
+        <v>798</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2170,7 +2170,7 @@
         <v>15</v>
       </c>
       <c r="B40" s="4">
-        <v>23</v>
+        <v>17609</v>
       </c>
       <c r="C40" s="4">
         <v>0</v>
@@ -2185,10 +2185,10 @@
         <v>0</v>
       </c>
       <c r="G40" s="4">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="H40" s="4">
-        <v>-16</v>
+        <v>-38</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -2196,7 +2196,7 @@
         <v>16</v>
       </c>
       <c r="B41" s="4">
-        <v>237</v>
+        <v>6014</v>
       </c>
       <c r="C41" s="4">
         <v>0</v>
@@ -2211,10 +2211,10 @@
         <v>0</v>
       </c>
       <c r="G41" s="4">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="H41" s="4">
-        <v>-139</v>
+        <v>-23</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -2222,13 +2222,13 @@
         <v>17</v>
       </c>
       <c r="B42" s="4">
-        <v>498</v>
+        <v>129061</v>
       </c>
       <c r="C42" s="4">
         <v>1</v>
       </c>
       <c r="D42" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E42" s="4">
         <v>0</v>
@@ -2237,10 +2237,10 @@
         <v>0</v>
       </c>
       <c r="G42" s="4">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="H42" s="4">
-        <v>759</v>
+        <v>828</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -2248,13 +2248,13 @@
         <v>18</v>
       </c>
       <c r="B43" s="4">
-        <v>432</v>
+        <v>960</v>
       </c>
       <c r="C43" s="4">
         <v>1</v>
       </c>
       <c r="D43" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E43" s="4">
         <v>0</v>
@@ -2263,10 +2263,10 @@
         <v>0</v>
       </c>
       <c r="G43" s="4">
-        <v>89</v>
+        <v>4</v>
       </c>
       <c r="H43" s="4">
-        <v>869</v>
+        <v>994</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -2274,13 +2274,13 @@
         <v>19</v>
       </c>
       <c r="B44" s="4">
-        <v>216</v>
+        <v>5795</v>
       </c>
       <c r="C44" s="4">
         <v>1</v>
       </c>
       <c r="D44" s="4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E44" s="4">
         <v>0</v>
@@ -2289,10 +2289,10 @@
         <v>0</v>
       </c>
       <c r="G44" s="4">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="H44" s="4">
-        <v>922</v>
+        <v>972</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -2300,7 +2300,7 @@
         <v>20</v>
       </c>
       <c r="B45" s="4">
-        <v>112</v>
+        <v>32871</v>
       </c>
       <c r="C45" s="4">
         <v>1</v>
@@ -2315,10 +2315,10 @@
         <v>0</v>
       </c>
       <c r="G45" s="4">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="H45" s="4">
-        <v>939</v>
+        <v>890</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -2364,13 +2364,13 @@
         <v>1</v>
       </c>
       <c r="B49" s="5">
-        <v>517</v>
+        <v>13419</v>
       </c>
       <c r="C49" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D49" s="5">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E49" s="5">
         <v>0</v>
@@ -2379,10 +2379,10 @@
         <v>0</v>
       </c>
       <c r="G49" s="5">
-        <v>102</v>
+        <v>11</v>
       </c>
       <c r="H49" s="5">
-        <v>883</v>
+        <v>-34</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -2390,13 +2390,13 @@
         <v>2</v>
       </c>
       <c r="B50" s="5">
-        <v>1040</v>
+        <v>97527</v>
       </c>
       <c r="C50" s="5">
         <v>1</v>
       </c>
       <c r="D50" s="5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E50" s="5">
         <v>0</v>
@@ -2405,10 +2405,10 @@
         <v>0</v>
       </c>
       <c r="G50" s="5">
-        <v>217</v>
+        <v>186</v>
       </c>
       <c r="H50" s="5">
-        <v>551</v>
+        <v>725</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -2416,10 +2416,10 @@
         <v>3</v>
       </c>
       <c r="B51" s="5">
-        <v>50</v>
+        <v>68311</v>
       </c>
       <c r="C51" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51" s="5">
         <v>0</v>
@@ -2431,10 +2431,10 @@
         <v>0</v>
       </c>
       <c r="G51" s="5">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="H51" s="5">
-        <v>-28</v>
+        <v>901</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -2442,10 +2442,10 @@
         <v>4</v>
       </c>
       <c r="B52" s="5">
-        <v>408</v>
+        <v>8567</v>
       </c>
       <c r="C52" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D52" s="5">
         <v>0</v>
@@ -2457,10 +2457,10 @@
         <v>0</v>
       </c>
       <c r="G52" s="5">
-        <v>81</v>
+        <v>9</v>
       </c>
       <c r="H52" s="5">
-        <v>802</v>
+        <v>-27</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -2468,10 +2468,10 @@
         <v>5</v>
       </c>
       <c r="B53" s="5">
-        <v>23</v>
+        <v>99006</v>
       </c>
       <c r="C53" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53" s="5">
         <v>0</v>
@@ -2483,10 +2483,10 @@
         <v>0</v>
       </c>
       <c r="G53" s="5">
-        <v>5</v>
+        <v>78</v>
       </c>
       <c r="H53" s="5">
-        <v>-16</v>
+        <v>808</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -2494,13 +2494,13 @@
         <v>6</v>
       </c>
       <c r="B54" s="5">
-        <v>950</v>
+        <v>41450</v>
       </c>
       <c r="C54" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D54" s="5">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E54" s="5">
         <v>0</v>
@@ -2509,10 +2509,10 @@
         <v>0</v>
       </c>
       <c r="G54" s="5">
-        <v>197</v>
+        <v>14</v>
       </c>
       <c r="H54" s="5">
-        <v>668</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -2520,10 +2520,10 @@
         <v>7</v>
       </c>
       <c r="B55" s="5">
-        <v>23</v>
+        <v>180642</v>
       </c>
       <c r="C55" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D55" s="5">
         <v>0</v>
@@ -2535,10 +2535,10 @@
         <v>0</v>
       </c>
       <c r="G55" s="5">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="H55" s="5">
-        <v>-16</v>
+        <v>749</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -2546,13 +2546,13 @@
         <v>8</v>
       </c>
       <c r="B56" s="5">
-        <v>161</v>
+        <v>94712</v>
       </c>
       <c r="C56" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D56" s="5">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E56" s="5">
         <v>0</v>
@@ -2561,10 +2561,10 @@
         <v>0</v>
       </c>
       <c r="G56" s="5">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="H56" s="5">
-        <v>-92</v>
+        <v>928</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -2572,13 +2572,13 @@
         <v>9</v>
       </c>
       <c r="B57" s="5">
-        <v>587</v>
+        <v>2774</v>
       </c>
       <c r="C57" s="5">
         <v>1</v>
       </c>
       <c r="D57" s="5">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E57" s="5">
         <v>0</v>
@@ -2587,10 +2587,10 @@
         <v>0</v>
       </c>
       <c r="G57" s="5">
-        <v>120</v>
+        <v>10</v>
       </c>
       <c r="H57" s="5">
-        <v>811</v>
+        <v>986</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -2598,13 +2598,13 @@
         <v>10</v>
       </c>
       <c r="B58" s="5">
-        <v>169</v>
+        <v>182526</v>
       </c>
       <c r="C58" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D58" s="5">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E58" s="5">
         <v>0</v>
@@ -2613,10 +2613,10 @@
         <v>0</v>
       </c>
       <c r="G58" s="5">
-        <v>33</v>
+        <v>138</v>
       </c>
       <c r="H58" s="5">
-        <v>-108</v>
+        <v>746</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -2624,7 +2624,7 @@
         <v>11</v>
       </c>
       <c r="B59" s="5">
-        <v>942</v>
+        <v>121254</v>
       </c>
       <c r="C59" s="5">
         <v>1</v>
@@ -2639,10 +2639,10 @@
         <v>0</v>
       </c>
       <c r="G59" s="5">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="H59" s="5">
-        <v>778</v>
+        <v>690</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -2650,13 +2650,13 @@
         <v>12</v>
       </c>
       <c r="B60" s="5">
-        <v>490</v>
+        <v>164077</v>
       </c>
       <c r="C60" s="5">
         <v>1</v>
       </c>
       <c r="D60" s="5">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E60" s="5">
         <v>0</v>
@@ -2665,10 +2665,10 @@
         <v>0</v>
       </c>
       <c r="G60" s="5">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="H60" s="5">
-        <v>856</v>
+        <v>654</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -2676,7 +2676,7 @@
         <v>13</v>
       </c>
       <c r="B61" s="5">
-        <v>118</v>
+        <v>71173</v>
       </c>
       <c r="C61" s="5">
         <v>1</v>
@@ -2691,10 +2691,10 @@
         <v>0</v>
       </c>
       <c r="G61" s="5">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="H61" s="5">
-        <v>946</v>
+        <v>840</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -2702,7 +2702,7 @@
         <v>14</v>
       </c>
       <c r="B62" s="5">
-        <v>955</v>
+        <v>104179</v>
       </c>
       <c r="C62" s="5">
         <v>1</v>
@@ -2717,10 +2717,10 @@
         <v>0</v>
       </c>
       <c r="G62" s="5">
-        <v>196</v>
+        <v>91</v>
       </c>
       <c r="H62" s="5">
-        <v>416</v>
+        <v>764</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -2728,7 +2728,7 @@
         <v>15</v>
       </c>
       <c r="B63" s="5">
-        <v>598</v>
+        <v>31803</v>
       </c>
       <c r="C63" s="5">
         <v>1</v>
@@ -2743,10 +2743,10 @@
         <v>0</v>
       </c>
       <c r="G63" s="5">
-        <v>119</v>
+        <v>24</v>
       </c>
       <c r="H63" s="5">
-        <v>677</v>
+        <v>946</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -2754,7 +2754,7 @@
         <v>16</v>
       </c>
       <c r="B64" s="5">
-        <v>73</v>
+        <v>6014</v>
       </c>
       <c r="C64" s="5">
         <v>0</v>
@@ -2769,10 +2769,10 @@
         <v>0</v>
       </c>
       <c r="G64" s="5">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H64" s="5">
-        <v>-36</v>
+        <v>-23</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -2780,13 +2780,13 @@
         <v>17</v>
       </c>
       <c r="B65" s="5">
-        <v>495</v>
+        <v>60866</v>
       </c>
       <c r="C65" s="5">
         <v>1</v>
       </c>
       <c r="D65" s="5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E65" s="5">
         <v>0</v>
@@ -2795,10 +2795,10 @@
         <v>0</v>
       </c>
       <c r="G65" s="5">
-        <v>98</v>
+        <v>218</v>
       </c>
       <c r="H65" s="5">
-        <v>847</v>
+        <v>662</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -2806,13 +2806,13 @@
         <v>18</v>
       </c>
       <c r="B66" s="5">
-        <v>331</v>
+        <v>192015</v>
       </c>
       <c r="C66" s="5">
         <v>1</v>
       </c>
       <c r="D66" s="5">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E66" s="5">
         <v>0</v>
@@ -2821,10 +2821,10 @@
         <v>0</v>
       </c>
       <c r="G66" s="5">
-        <v>64</v>
+        <v>190</v>
       </c>
       <c r="H66" s="5">
-        <v>835</v>
+        <v>636</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -2832,13 +2832,13 @@
         <v>19</v>
       </c>
       <c r="B67" s="5">
-        <v>23</v>
+        <v>174272</v>
       </c>
       <c r="C67" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D67" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E67" s="5">
         <v>0</v>
@@ -2847,10 +2847,10 @@
         <v>0</v>
       </c>
       <c r="G67" s="5">
-        <v>5</v>
+        <v>207</v>
       </c>
       <c r="H67" s="5">
-        <v>-16</v>
+        <v>500</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -2858,13 +2858,13 @@
         <v>20</v>
       </c>
       <c r="B68" s="5">
-        <v>58</v>
+        <v>131661</v>
       </c>
       <c r="C68" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D68" s="5">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E68" s="5">
         <v>0</v>
@@ -2873,10 +2873,10 @@
         <v>0</v>
       </c>
       <c r="G68" s="5">
-        <v>10</v>
+        <v>155</v>
       </c>
       <c r="H68" s="5">
-        <v>-26</v>
+        <v>784</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -2922,13 +2922,13 @@
         <v>1</v>
       </c>
       <c r="B72" s="5">
-        <v>1674</v>
+        <v>226790</v>
       </c>
       <c r="C72" s="5">
         <v>1</v>
       </c>
       <c r="D72" s="5">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E72" s="5">
         <v>0</v>
@@ -2937,10 +2937,10 @@
         <v>0</v>
       </c>
       <c r="G72" s="5">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="H72" s="5">
-        <v>467</v>
+        <v>500</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -2948,13 +2948,13 @@
         <v>2</v>
       </c>
       <c r="B73" s="5">
-        <v>968</v>
+        <v>73895</v>
       </c>
       <c r="C73" s="5">
         <v>1</v>
       </c>
       <c r="D73" s="5">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E73" s="5">
         <v>0</v>
@@ -2963,10 +2963,10 @@
         <v>0</v>
       </c>
       <c r="G73" s="5">
-        <v>195</v>
+        <v>371</v>
       </c>
       <c r="H73" s="5">
-        <v>857</v>
+        <v>503</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -2974,13 +2974,13 @@
         <v>3</v>
       </c>
       <c r="B74" s="5">
-        <v>865</v>
+        <v>83343</v>
       </c>
       <c r="C74" s="5">
         <v>1</v>
       </c>
       <c r="D74" s="5">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E74" s="5">
         <v>0</v>
@@ -2989,10 +2989,10 @@
         <v>0</v>
       </c>
       <c r="G74" s="5">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H74" s="5">
-        <v>674</v>
+        <v>841</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -3000,7 +3000,7 @@
         <v>4</v>
       </c>
       <c r="B75" s="5">
-        <v>746</v>
+        <v>46027</v>
       </c>
       <c r="C75" s="5">
         <v>1</v>
@@ -3015,10 +3015,10 @@
         <v>0</v>
       </c>
       <c r="G75" s="5">
-        <v>151</v>
+        <v>57</v>
       </c>
       <c r="H75" s="5">
-        <v>658</v>
+        <v>893</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -3026,7 +3026,7 @@
         <v>5</v>
       </c>
       <c r="B76" s="5">
-        <v>80</v>
+        <v>30259</v>
       </c>
       <c r="C76" s="5">
         <v>0</v>
@@ -3041,10 +3041,10 @@
         <v>0</v>
       </c>
       <c r="G76" s="5">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H76" s="5">
-        <v>-57</v>
+        <v>-26</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -3052,13 +3052,13 @@
         <v>6</v>
       </c>
       <c r="B77" s="5">
-        <v>919</v>
+        <v>224075</v>
       </c>
       <c r="C77" s="5">
         <v>1</v>
       </c>
       <c r="D77" s="5">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E77" s="5">
         <v>0</v>
@@ -3067,10 +3067,10 @@
         <v>0</v>
       </c>
       <c r="G77" s="5">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="H77" s="5">
-        <v>796</v>
+        <v>625</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -3078,7 +3078,7 @@
         <v>7</v>
       </c>
       <c r="B78" s="5">
-        <v>158</v>
+        <v>4818</v>
       </c>
       <c r="C78" s="5">
         <v>0</v>
@@ -3093,10 +3093,10 @@
         <v>0</v>
       </c>
       <c r="G78" s="5">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="H78" s="5">
-        <v>-95</v>
+        <v>-16</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -3104,13 +3104,13 @@
         <v>8</v>
       </c>
       <c r="B79" s="5">
-        <v>44</v>
+        <v>226804</v>
       </c>
       <c r="C79" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D79" s="5">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E79" s="5">
         <v>0</v>
@@ -3119,10 +3119,10 @@
         <v>0</v>
       </c>
       <c r="G79" s="5">
-        <v>8</v>
+        <v>324</v>
       </c>
       <c r="H79" s="5">
-        <v>-25</v>
+        <v>555</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -3130,10 +3130,10 @@
         <v>9</v>
       </c>
       <c r="B80" s="5">
-        <v>293</v>
+        <v>68034</v>
       </c>
       <c r="C80" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D80" s="5">
         <v>0</v>
@@ -3145,10 +3145,10 @@
         <v>0</v>
       </c>
       <c r="G80" s="5">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="H80" s="5">
-        <v>886</v>
+        <v>-99</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -3156,7 +3156,7 @@
         <v>10</v>
       </c>
       <c r="B81" s="5">
-        <v>63</v>
+        <v>29376</v>
       </c>
       <c r="C81" s="5">
         <v>0</v>
@@ -3171,10 +3171,10 @@
         <v>0</v>
       </c>
       <c r="G81" s="5">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H81" s="5">
-        <v>-28</v>
+        <v>-41</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -3182,13 +3182,13 @@
         <v>11</v>
       </c>
       <c r="B82" s="5">
-        <v>23</v>
+        <v>125152</v>
       </c>
       <c r="C82" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D82" s="5">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E82" s="5">
         <v>0</v>
@@ -3197,10 +3197,10 @@
         <v>0</v>
       </c>
       <c r="G82" s="5">
-        <v>5</v>
+        <v>383</v>
       </c>
       <c r="H82" s="5">
-        <v>-16</v>
+        <v>484</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -3208,13 +3208,13 @@
         <v>12</v>
       </c>
       <c r="B83" s="5">
-        <v>116</v>
+        <v>32027</v>
       </c>
       <c r="C83" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D83" s="5">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E83" s="5">
         <v>0</v>
@@ -3223,10 +3223,10 @@
         <v>0</v>
       </c>
       <c r="G83" s="5">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="H83" s="5">
-        <v>-72</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -3234,13 +3234,13 @@
         <v>13</v>
       </c>
       <c r="B84" s="5">
-        <v>1759</v>
+        <v>122103</v>
       </c>
       <c r="C84" s="5">
         <v>1</v>
       </c>
       <c r="D84" s="5">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E84" s="5">
         <v>0</v>
@@ -3249,10 +3249,10 @@
         <v>0</v>
       </c>
       <c r="G84" s="5">
-        <v>354</v>
+        <v>411</v>
       </c>
       <c r="H84" s="5">
-        <v>371</v>
+        <v>359</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -3260,10 +3260,10 @@
         <v>14</v>
       </c>
       <c r="B85" s="5">
-        <v>552</v>
+        <v>11370</v>
       </c>
       <c r="C85" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D85" s="5">
         <v>0</v>
@@ -3275,10 +3275,10 @@
         <v>0</v>
       </c>
       <c r="G85" s="5">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="H85" s="5">
-        <v>701</v>
+        <v>-25</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -3286,13 +3286,13 @@
         <v>15</v>
       </c>
       <c r="B86" s="5">
-        <v>23</v>
+        <v>144680</v>
       </c>
       <c r="C86" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D86" s="5">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E86" s="5">
         <v>0</v>
@@ -3301,10 +3301,10 @@
         <v>0</v>
       </c>
       <c r="G86" s="5">
-        <v>5</v>
+        <v>373</v>
       </c>
       <c r="H86" s="5">
-        <v>-16</v>
+        <v>495</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -3312,10 +3312,10 @@
         <v>16</v>
       </c>
       <c r="B87" s="5">
-        <v>214</v>
+        <v>6110</v>
       </c>
       <c r="C87" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D87" s="5">
         <v>0</v>
@@ -3327,10 +3327,10 @@
         <v>0</v>
       </c>
       <c r="G87" s="5">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="H87" s="5">
-        <v>925</v>
+        <v>-16</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -3338,13 +3338,13 @@
         <v>17</v>
       </c>
       <c r="B88" s="5">
-        <v>221</v>
+        <v>102528</v>
       </c>
       <c r="C88" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D88" s="5">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E88" s="5">
         <v>0</v>
@@ -3353,10 +3353,10 @@
         <v>0</v>
       </c>
       <c r="G88" s="5">
-        <v>43</v>
+        <v>319</v>
       </c>
       <c r="H88" s="5">
-        <v>-144</v>
+        <v>600</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -3364,13 +3364,13 @@
         <v>18</v>
       </c>
       <c r="B89" s="5">
-        <v>64</v>
+        <v>54333</v>
       </c>
       <c r="C89" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D89" s="5">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E89" s="5">
         <v>0</v>
@@ -3379,10 +3379,10 @@
         <v>0</v>
       </c>
       <c r="G89" s="5">
-        <v>12</v>
+        <v>149</v>
       </c>
       <c r="H89" s="5">
-        <v>-31</v>
+        <v>877</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -3390,10 +3390,10 @@
         <v>19</v>
       </c>
       <c r="B90" s="5">
-        <v>308</v>
+        <v>22491</v>
       </c>
       <c r="C90" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D90" s="5">
         <v>0</v>
@@ -3405,10 +3405,10 @@
         <v>0</v>
       </c>
       <c r="G90" s="5">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="H90" s="5">
-        <v>898</v>
+        <v>-68</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -3416,13 +3416,13 @@
         <v>20</v>
       </c>
       <c r="B91" s="5">
-        <v>1137</v>
+        <v>271490</v>
       </c>
       <c r="C91" s="5">
         <v>1</v>
       </c>
       <c r="D91" s="5">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E91" s="5">
         <v>0</v>
@@ -3431,10 +3431,10 @@
         <v>0</v>
       </c>
       <c r="G91" s="5">
-        <v>232</v>
+        <v>330</v>
       </c>
       <c r="H91" s="5">
-        <v>825</v>
+        <v>420</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -3480,13 +3480,13 @@
         <v>1</v>
       </c>
       <c r="B95" s="5">
-        <v>1033</v>
+        <v>87467</v>
       </c>
       <c r="C95" s="5">
         <v>1</v>
       </c>
       <c r="D95" s="5">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E95" s="5">
         <v>0</v>
@@ -3495,10 +3495,10 @@
         <v>0</v>
       </c>
       <c r="G95" s="5">
-        <v>210</v>
+        <v>278</v>
       </c>
       <c r="H95" s="5">
-        <v>772</v>
+        <v>724</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -3506,13 +3506,13 @@
         <v>2</v>
       </c>
       <c r="B96" s="5">
-        <v>862</v>
+        <v>121980</v>
       </c>
       <c r="C96" s="5">
         <v>1</v>
       </c>
       <c r="D96" s="5">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E96" s="5">
         <v>0</v>
@@ -3521,10 +3521,10 @@
         <v>0</v>
       </c>
       <c r="G96" s="5">
-        <v>175</v>
+        <v>101</v>
       </c>
       <c r="H96" s="5">
-        <v>938</v>
+        <v>793</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -3532,25 +3532,25 @@
         <v>3</v>
       </c>
       <c r="B97" s="5">
-        <v>2214</v>
+        <v>20948</v>
       </c>
       <c r="C97" s="5">
         <v>1</v>
       </c>
       <c r="D97" s="5">
+        <v>0</v>
+      </c>
+      <c r="E97" s="5">
+        <v>0</v>
+      </c>
+      <c r="F97" s="5">
+        <v>0</v>
+      </c>
+      <c r="G97" s="5">
         <v>14</v>
       </c>
-      <c r="E97" s="5">
-        <v>0</v>
-      </c>
-      <c r="F97" s="5">
-        <v>0</v>
-      </c>
-      <c r="G97" s="5">
-        <v>453</v>
-      </c>
       <c r="H97" s="5">
-        <v>475</v>
+        <v>957</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -3558,13 +3558,13 @@
         <v>4</v>
       </c>
       <c r="B98" s="5">
-        <v>712</v>
+        <v>16711</v>
       </c>
       <c r="C98" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D98" s="5">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E98" s="5">
         <v>0</v>
@@ -3573,10 +3573,10 @@
         <v>0</v>
       </c>
       <c r="G98" s="5">
-        <v>145</v>
+        <v>11</v>
       </c>
       <c r="H98" s="5">
-        <v>910</v>
+        <v>-34</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -3584,13 +3584,13 @@
         <v>5</v>
       </c>
       <c r="B99" s="5">
-        <v>689</v>
+        <v>60319</v>
       </c>
       <c r="C99" s="5">
         <v>1</v>
       </c>
       <c r="D99" s="5">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E99" s="5">
         <v>0</v>
@@ -3599,10 +3599,10 @@
         <v>0</v>
       </c>
       <c r="G99" s="5">
-        <v>140</v>
+        <v>490</v>
       </c>
       <c r="H99" s="5">
-        <v>845</v>
+        <v>442</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -3610,13 +3610,13 @@
         <v>6</v>
       </c>
       <c r="B100" s="5">
-        <v>522</v>
+        <v>112040</v>
       </c>
       <c r="C100" s="5">
         <v>1</v>
       </c>
       <c r="D100" s="5">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E100" s="5">
         <v>0</v>
@@ -3625,10 +3625,10 @@
         <v>0</v>
       </c>
       <c r="G100" s="5">
-        <v>103</v>
+        <v>288</v>
       </c>
       <c r="H100" s="5">
-        <v>793</v>
+        <v>612</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -3636,13 +3636,13 @@
         <v>7</v>
       </c>
       <c r="B101" s="5">
-        <v>1558</v>
+        <v>69434</v>
       </c>
       <c r="C101" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D101" s="5">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E101" s="5">
         <v>0</v>
@@ -3651,10 +3651,10 @@
         <v>0</v>
       </c>
       <c r="G101" s="5">
-        <v>315</v>
+        <v>35</v>
       </c>
       <c r="H101" s="5">
-        <v>715</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -3662,13 +3662,13 @@
         <v>8</v>
       </c>
       <c r="B102" s="5">
-        <v>62</v>
+        <v>72424</v>
       </c>
       <c r="C102" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D102" s="5">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E102" s="5">
         <v>0</v>
@@ -3677,10 +3677,10 @@
         <v>0</v>
       </c>
       <c r="G102" s="5">
-        <v>12</v>
+        <v>385</v>
       </c>
       <c r="H102" s="5">
-        <v>-36</v>
+        <v>595</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -3688,13 +3688,13 @@
         <v>9</v>
       </c>
       <c r="B103" s="5">
-        <v>48</v>
+        <v>278034</v>
       </c>
       <c r="C103" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D103" s="5">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E103" s="5">
         <v>0</v>
@@ -3703,10 +3703,10 @@
         <v>0</v>
       </c>
       <c r="G103" s="5">
-        <v>10</v>
+        <v>476</v>
       </c>
       <c r="H103" s="5">
-        <v>-32</v>
+        <v>278</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -3714,10 +3714,10 @@
         <v>10</v>
       </c>
       <c r="B104" s="5">
-        <v>1068</v>
+        <v>2842</v>
       </c>
       <c r="C104" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D104" s="5">
         <v>0</v>
@@ -3729,10 +3729,10 @@
         <v>0</v>
       </c>
       <c r="G104" s="5">
-        <v>213</v>
+        <v>5</v>
       </c>
       <c r="H104" s="5">
-        <v>569</v>
+        <v>-16</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -3740,13 +3740,13 @@
         <v>11</v>
       </c>
       <c r="B105" s="5">
-        <v>1662</v>
+        <v>174681</v>
       </c>
       <c r="C105" s="5">
         <v>1</v>
       </c>
       <c r="D105" s="5">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E105" s="5">
         <v>0</v>
@@ -3755,10 +3755,10 @@
         <v>0</v>
       </c>
       <c r="G105" s="5">
-        <v>339</v>
+        <v>229</v>
       </c>
       <c r="H105" s="5">
-        <v>374</v>
+        <v>634</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -3766,10 +3766,10 @@
         <v>12</v>
       </c>
       <c r="B106" s="5">
-        <v>931</v>
+        <v>28613</v>
       </c>
       <c r="C106" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D106" s="5">
         <v>0</v>
@@ -3781,10 +3781,10 @@
         <v>0</v>
       </c>
       <c r="G106" s="5">
-        <v>190</v>
+        <v>14</v>
       </c>
       <c r="H106" s="5">
-        <v>693</v>
+        <v>-38</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -3792,10 +3792,10 @@
         <v>13</v>
       </c>
       <c r="B107" s="5">
-        <v>275</v>
+        <v>19226</v>
       </c>
       <c r="C107" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D107" s="5">
         <v>0</v>
@@ -3807,10 +3807,10 @@
         <v>0</v>
       </c>
       <c r="G107" s="5">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="H107" s="5">
-        <v>871</v>
+        <v>-34</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -3818,7 +3818,7 @@
         <v>14</v>
       </c>
       <c r="B108" s="5">
-        <v>2187</v>
+        <v>55685</v>
       </c>
       <c r="C108" s="5">
         <v>1</v>
@@ -3833,10 +3833,10 @@
         <v>0</v>
       </c>
       <c r="G108" s="5">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="H108" s="5">
-        <v>509</v>
+        <v>551</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -3844,10 +3844,10 @@
         <v>15</v>
       </c>
       <c r="B109" s="5">
-        <v>1192</v>
+        <v>27401</v>
       </c>
       <c r="C109" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D109" s="5">
         <v>0</v>
@@ -3859,10 +3859,10 @@
         <v>0</v>
       </c>
       <c r="G109" s="5">
-        <v>241</v>
+        <v>16</v>
       </c>
       <c r="H109" s="5">
-        <v>551</v>
+        <v>-58</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -3870,13 +3870,13 @@
         <v>16</v>
       </c>
       <c r="B110" s="5">
-        <v>1745</v>
+        <v>142431</v>
       </c>
       <c r="C110" s="5">
         <v>1</v>
       </c>
       <c r="D110" s="5">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E110" s="5">
         <v>0</v>
@@ -3885,10 +3885,10 @@
         <v>0</v>
       </c>
       <c r="G110" s="5">
-        <v>356</v>
+        <v>458</v>
       </c>
       <c r="H110" s="5">
-        <v>524</v>
+        <v>528</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -3896,7 +3896,7 @@
         <v>17</v>
       </c>
       <c r="B111" s="5">
-        <v>131</v>
+        <v>6021</v>
       </c>
       <c r="C111" s="5">
         <v>0</v>
@@ -3911,10 +3911,10 @@
         <v>0</v>
       </c>
       <c r="G111" s="5">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="H111" s="5">
-        <v>-70</v>
+        <v>-24</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -3922,13 +3922,13 @@
         <v>18</v>
       </c>
       <c r="B112" s="5">
-        <v>39</v>
+        <v>279884</v>
       </c>
       <c r="C112" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D112" s="5">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="E112" s="5">
         <v>0</v>
@@ -3937,10 +3937,10 @@
         <v>0</v>
       </c>
       <c r="G112" s="5">
-        <v>7</v>
+        <v>529</v>
       </c>
       <c r="H112" s="5">
-        <v>-19</v>
+        <v>177</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -3948,13 +3948,13 @@
         <v>19</v>
       </c>
       <c r="B113" s="5">
-        <v>2208</v>
+        <v>44296</v>
       </c>
       <c r="C113" s="5">
         <v>1</v>
       </c>
       <c r="D113" s="5">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E113" s="5">
         <v>0</v>
@@ -3963,10 +3963,10 @@
         <v>0</v>
       </c>
       <c r="G113" s="5">
-        <v>455</v>
+        <v>99</v>
       </c>
       <c r="H113" s="5">
-        <v>445</v>
+        <v>823</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -3974,13 +3974,13 @@
         <v>20</v>
       </c>
       <c r="B114" s="5">
-        <v>439</v>
+        <v>24768</v>
       </c>
       <c r="C114" s="5">
         <v>1</v>
       </c>
       <c r="D114" s="5">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E114" s="5">
         <v>0</v>
@@ -3989,10 +3989,10 @@
         <v>0</v>
       </c>
       <c r="G114" s="5">
-        <v>88</v>
+        <v>32</v>
       </c>
       <c r="H114" s="5">
-        <v>1073</v>
+        <v>939</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added lots of statistics outputs
</commit_message>
<xml_diff>
--- a/CSCI446_Project2_WumpusWorld/references/statistics/AgentRunStatistics.xlsx
+++ b/CSCI446_Project2_WumpusWorld/references/statistics/AgentRunStatistics.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reactive Agent" sheetId="1" r:id="rId1"/>
     <sheet name="Knowledge Based Agent" sheetId="3" r:id="rId2"/>
+    <sheet name="KB-Decisions Made Graphs" sheetId="4" r:id="rId3"/>
+    <sheet name="KB-Points Graph" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="25">
   <si>
     <t>Map Size: 5x5</t>
   </si>
@@ -73,6 +75,33 @@
   </si>
   <si>
     <t>Score</t>
+  </si>
+  <si>
+    <t>5x5</t>
+  </si>
+  <si>
+    <t>Size:</t>
+  </si>
+  <si>
+    <t>Average:</t>
+  </si>
+  <si>
+    <t>10x10</t>
+  </si>
+  <si>
+    <t>15x15</t>
+  </si>
+  <si>
+    <t>20x20</t>
+  </si>
+  <si>
+    <t>25x25</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>Avg:</t>
   </si>
 </sst>
 </file>
@@ -198,6 +227,2167 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>KB-Agent: Avgerage Decisions Made</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10891426071741032"/>
+          <c:y val="0.15042833187518226"/>
+          <c:w val="0.85219685039370074"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>15</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>20</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>25</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'KB-Decisions Made Graphs'!$B$23:$F$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8569.7000000000007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53311.199999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>92312.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95285.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>82260.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-1109161248"/>
+        <c:axId val="-1109174304"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-1109161248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>World</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> size</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1109174304"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1109174304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Decisions made</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1109161248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>KB-Agent: Score</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>15</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>20</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>25</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'KB-Points Graph'!$B$23:$F$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>722.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>607</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>609.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>396.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>387.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-1109169952"/>
+        <c:axId val="-1109173216"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-1109169952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>World Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1109173216"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1109173216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Points Earned</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1109169952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1057275</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4761</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>176211</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1187,10 +3377,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H114"/>
+  <dimension ref="A1:H115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="J107" sqref="J107"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1763,6 +3953,39 @@
         <v>981</v>
       </c>
     </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <f t="shared" ref="B23:H23" si="0">AVERAGE(B3:B22)</f>
+        <v>8569.7000000000007</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>12.2</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>722.2</v>
+      </c>
+    </row>
     <row r="24" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>9</v>
@@ -2321,6 +4544,39 @@
         <v>890</v>
       </c>
     </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46">
+        <f t="shared" ref="B46:H46" si="1">AVERAGE(B26:B45)</f>
+        <v>53311.199999999997</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="1"/>
+        <v>1.8</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="1"/>
+        <v>44.9</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="1"/>
+        <v>607</v>
+      </c>
+    </row>
     <row r="47" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
         <v>10</v>
@@ -2879,6 +5135,39 @@
         <v>784</v>
       </c>
     </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>24</v>
+      </c>
+      <c r="B69">
+        <f t="shared" ref="B69:H69" si="2">AVERAGE(B49:B68)</f>
+        <v>92312.4</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="2"/>
+        <v>3.45</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="2"/>
+        <v>609.75</v>
+      </c>
+    </row>
     <row r="70" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A70" s="9" t="s">
         <v>11</v>
@@ -3437,6 +5726,39 @@
         <v>420</v>
       </c>
     </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>24</v>
+      </c>
+      <c r="B92">
+        <f t="shared" ref="B92:H92" si="3">AVERAGE(B72:B91)</f>
+        <v>95285.25</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="3"/>
+        <v>0.65</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="3"/>
+        <v>7.6</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F92">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G92">
+        <f t="shared" si="3"/>
+        <v>177.5</v>
+      </c>
+      <c r="H92">
+        <f t="shared" si="3"/>
+        <v>396.8</v>
+      </c>
+    </row>
     <row r="93" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A93" s="9" t="s">
         <v>12</v>
@@ -3993,6 +6315,39 @@
       </c>
       <c r="H114" s="5">
         <v>939</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>24</v>
+      </c>
+      <c r="B115">
+        <f t="shared" ref="B115:H115" si="4">AVERAGE(B95:B114)</f>
+        <v>82260.25</v>
+      </c>
+      <c r="C115">
+        <f t="shared" si="4"/>
+        <v>0.65</v>
+      </c>
+      <c r="D115">
+        <f t="shared" si="4"/>
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="E115">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F115">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G115">
+        <f t="shared" si="4"/>
+        <v>195.9</v>
+      </c>
+      <c r="H115">
+        <f t="shared" si="4"/>
+        <v>387.95</v>
       </c>
     </row>
   </sheetData>
@@ -4005,4 +6360,981 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>21411</v>
+      </c>
+      <c r="C3" s="4">
+        <v>13870</v>
+      </c>
+      <c r="D3" s="5">
+        <v>13419</v>
+      </c>
+      <c r="E3" s="5">
+        <v>226790</v>
+      </c>
+      <c r="F3" s="5">
+        <v>87467</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
+        <v>146</v>
+      </c>
+      <c r="C4" s="4">
+        <v>30041</v>
+      </c>
+      <c r="D4" s="5">
+        <v>97527</v>
+      </c>
+      <c r="E4" s="5">
+        <v>73895</v>
+      </c>
+      <c r="F4" s="5">
+        <v>121980</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>768</v>
+      </c>
+      <c r="C5" s="4">
+        <v>17121</v>
+      </c>
+      <c r="D5" s="5">
+        <v>68311</v>
+      </c>
+      <c r="E5" s="5">
+        <v>83343</v>
+      </c>
+      <c r="F5" s="5">
+        <v>20948</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1617</v>
+      </c>
+      <c r="C6" s="4">
+        <v>98899</v>
+      </c>
+      <c r="D6" s="5">
+        <v>8567</v>
+      </c>
+      <c r="E6" s="5">
+        <v>46027</v>
+      </c>
+      <c r="F6" s="5">
+        <v>16711</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4">
+        <v>18292</v>
+      </c>
+      <c r="C7" s="4">
+        <v>74683</v>
+      </c>
+      <c r="D7" s="5">
+        <v>99006</v>
+      </c>
+      <c r="E7" s="5">
+        <v>30259</v>
+      </c>
+      <c r="F7" s="5">
+        <v>60319</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4">
+        <v>10131</v>
+      </c>
+      <c r="C8" s="4">
+        <v>6110</v>
+      </c>
+      <c r="D8" s="5">
+        <v>41450</v>
+      </c>
+      <c r="E8" s="5">
+        <v>224075</v>
+      </c>
+      <c r="F8" s="5">
+        <v>112040</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4">
+        <v>768</v>
+      </c>
+      <c r="C9" s="4">
+        <v>88583</v>
+      </c>
+      <c r="D9" s="5">
+        <v>180642</v>
+      </c>
+      <c r="E9" s="5">
+        <v>4818</v>
+      </c>
+      <c r="F9" s="5">
+        <v>69434</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4">
+        <v>17114</v>
+      </c>
+      <c r="C10" s="4">
+        <v>98820</v>
+      </c>
+      <c r="D10" s="5">
+        <v>94712</v>
+      </c>
+      <c r="E10" s="5">
+        <v>226804</v>
+      </c>
+      <c r="F10" s="5">
+        <v>72424</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4">
+        <v>10871</v>
+      </c>
+      <c r="C11" s="4">
+        <v>67218</v>
+      </c>
+      <c r="D11" s="5">
+        <v>2774</v>
+      </c>
+      <c r="E11" s="5">
+        <v>68034</v>
+      </c>
+      <c r="F11" s="5">
+        <v>278034</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4">
+        <v>6529</v>
+      </c>
+      <c r="C12" s="4">
+        <v>17052</v>
+      </c>
+      <c r="D12" s="5">
+        <v>182526</v>
+      </c>
+      <c r="E12" s="5">
+        <v>29376</v>
+      </c>
+      <c r="F12" s="5">
+        <v>2842</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4">
+        <v>2301</v>
+      </c>
+      <c r="C13" s="4">
+        <v>109761</v>
+      </c>
+      <c r="D13" s="5">
+        <v>121254</v>
+      </c>
+      <c r="E13" s="5">
+        <v>125152</v>
+      </c>
+      <c r="F13" s="5">
+        <v>174681</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4">
+        <v>8342</v>
+      </c>
+      <c r="C14" s="4">
+        <v>109075</v>
+      </c>
+      <c r="D14" s="5">
+        <v>164077</v>
+      </c>
+      <c r="E14" s="5">
+        <v>32027</v>
+      </c>
+      <c r="F14" s="5">
+        <v>28613</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4">
+        <v>5832</v>
+      </c>
+      <c r="C15" s="4">
+        <v>33121</v>
+      </c>
+      <c r="D15" s="5">
+        <v>71173</v>
+      </c>
+      <c r="E15" s="5">
+        <v>122103</v>
+      </c>
+      <c r="F15" s="5">
+        <v>19226</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4">
+        <v>146</v>
+      </c>
+      <c r="C16" s="4">
+        <v>109560</v>
+      </c>
+      <c r="D16" s="5">
+        <v>104179</v>
+      </c>
+      <c r="E16" s="5">
+        <v>11370</v>
+      </c>
+      <c r="F16" s="5">
+        <v>55685</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17" s="4">
+        <v>24083</v>
+      </c>
+      <c r="C17" s="4">
+        <v>17609</v>
+      </c>
+      <c r="D17" s="5">
+        <v>31803</v>
+      </c>
+      <c r="E17" s="5">
+        <v>144680</v>
+      </c>
+      <c r="F17" s="5">
+        <v>27401</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4">
+        <v>9426</v>
+      </c>
+      <c r="C18" s="4">
+        <v>6014</v>
+      </c>
+      <c r="D18" s="5">
+        <v>6014</v>
+      </c>
+      <c r="E18" s="5">
+        <v>6110</v>
+      </c>
+      <c r="F18" s="5">
+        <v>142431</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4">
+        <v>15410</v>
+      </c>
+      <c r="C19" s="4">
+        <v>129061</v>
+      </c>
+      <c r="D19" s="5">
+        <v>60866</v>
+      </c>
+      <c r="E19" s="5">
+        <v>102528</v>
+      </c>
+      <c r="F19" s="5">
+        <v>6021</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20" s="4">
+        <v>4716</v>
+      </c>
+      <c r="C20" s="4">
+        <v>960</v>
+      </c>
+      <c r="D20" s="5">
+        <v>192015</v>
+      </c>
+      <c r="E20" s="5">
+        <v>54333</v>
+      </c>
+      <c r="F20" s="5">
+        <v>279884</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>19</v>
+      </c>
+      <c r="B21" s="4">
+        <v>8061</v>
+      </c>
+      <c r="C21" s="4">
+        <v>5795</v>
+      </c>
+      <c r="D21" s="5">
+        <v>174272</v>
+      </c>
+      <c r="E21" s="5">
+        <v>22491</v>
+      </c>
+      <c r="F21" s="5">
+        <v>44296</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="B22" s="4">
+        <v>5430</v>
+      </c>
+      <c r="C22" s="4">
+        <v>32871</v>
+      </c>
+      <c r="D22" s="5">
+        <v>131661</v>
+      </c>
+      <c r="E22" s="5">
+        <v>271490</v>
+      </c>
+      <c r="F22" s="5">
+        <v>24768</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23">
+        <f>AVERAGE(B3:B22)</f>
+        <v>8569.7000000000007</v>
+      </c>
+      <c r="C23">
+        <f>AVERAGE(C3:C22)</f>
+        <v>53311.199999999997</v>
+      </c>
+      <c r="D23">
+        <f>AVERAGE(D3:D22)</f>
+        <v>92312.4</v>
+      </c>
+      <c r="E23">
+        <f>AVERAGE(E3:E22)</f>
+        <v>95285.25</v>
+      </c>
+      <c r="F23">
+        <f>AVERAGE(F3:F22)</f>
+        <v>82260.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>-54</v>
+      </c>
+      <c r="C3" s="4">
+        <v>961</v>
+      </c>
+      <c r="D3" s="5">
+        <v>-34</v>
+      </c>
+      <c r="E3" s="5">
+        <v>500</v>
+      </c>
+      <c r="F3" s="5">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>938</v>
+      </c>
+      <c r="D4" s="5">
+        <v>725</v>
+      </c>
+      <c r="E4" s="5">
+        <v>503</v>
+      </c>
+      <c r="F4" s="5">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>-7</v>
+      </c>
+      <c r="C5" s="4">
+        <v>-32</v>
+      </c>
+      <c r="D5" s="5">
+        <v>901</v>
+      </c>
+      <c r="E5" s="5">
+        <v>841</v>
+      </c>
+      <c r="F5" s="5">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>989</v>
+      </c>
+      <c r="C6" s="4">
+        <v>797</v>
+      </c>
+      <c r="D6" s="5">
+        <v>-27</v>
+      </c>
+      <c r="E6" s="5">
+        <v>893</v>
+      </c>
+      <c r="F6" s="5">
+        <v>-34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4">
+        <v>954</v>
+      </c>
+      <c r="C7" s="4">
+        <v>853</v>
+      </c>
+      <c r="D7" s="5">
+        <v>808</v>
+      </c>
+      <c r="E7" s="5">
+        <v>-26</v>
+      </c>
+      <c r="F7" s="5">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4">
+        <v>976</v>
+      </c>
+      <c r="C8" s="4">
+        <v>-16</v>
+      </c>
+      <c r="D8" s="5">
+        <v>-40</v>
+      </c>
+      <c r="E8" s="5">
+        <v>625</v>
+      </c>
+      <c r="F8" s="5">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4">
+        <v>-7</v>
+      </c>
+      <c r="C9" s="4">
+        <v>912</v>
+      </c>
+      <c r="D9" s="5">
+        <v>749</v>
+      </c>
+      <c r="E9" s="5">
+        <v>-16</v>
+      </c>
+      <c r="F9" s="5">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4">
+        <v>960</v>
+      </c>
+      <c r="C10" s="4">
+        <v>785</v>
+      </c>
+      <c r="D10" s="5">
+        <v>928</v>
+      </c>
+      <c r="E10" s="5">
+        <v>555</v>
+      </c>
+      <c r="F10" s="5">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4">
+        <v>954</v>
+      </c>
+      <c r="C11" s="4">
+        <v>838</v>
+      </c>
+      <c r="D11" s="5">
+        <v>986</v>
+      </c>
+      <c r="E11" s="5">
+        <v>-99</v>
+      </c>
+      <c r="F11" s="5">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4">
+        <v>968</v>
+      </c>
+      <c r="C12" s="4">
+        <v>-28</v>
+      </c>
+      <c r="D12" s="5">
+        <v>746</v>
+      </c>
+      <c r="E12" s="5">
+        <v>-41</v>
+      </c>
+      <c r="F12" s="5">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4">
+        <v>991</v>
+      </c>
+      <c r="C13" s="4">
+        <v>901</v>
+      </c>
+      <c r="D13" s="5">
+        <v>690</v>
+      </c>
+      <c r="E13" s="5">
+        <v>484</v>
+      </c>
+      <c r="F13" s="5">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4">
+        <v>970</v>
+      </c>
+      <c r="C14" s="4">
+        <v>861</v>
+      </c>
+      <c r="D14" s="5">
+        <v>654</v>
+      </c>
+      <c r="E14" s="5">
+        <v>1075</v>
+      </c>
+      <c r="F14" s="5">
+        <v>-38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4">
+        <v>977</v>
+      </c>
+      <c r="C15" s="4">
+        <v>-51</v>
+      </c>
+      <c r="D15" s="5">
+        <v>840</v>
+      </c>
+      <c r="E15" s="5">
+        <v>359</v>
+      </c>
+      <c r="F15" s="5">
+        <v>-34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>798</v>
+      </c>
+      <c r="D16" s="5">
+        <v>764</v>
+      </c>
+      <c r="E16" s="5">
+        <v>-25</v>
+      </c>
+      <c r="F16" s="5">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17" s="4">
+        <v>944</v>
+      </c>
+      <c r="C17" s="4">
+        <v>-38</v>
+      </c>
+      <c r="D17" s="5">
+        <v>946</v>
+      </c>
+      <c r="E17" s="5">
+        <v>495</v>
+      </c>
+      <c r="F17" s="5">
+        <v>-58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4">
+        <v>958</v>
+      </c>
+      <c r="C18" s="4">
+        <v>-23</v>
+      </c>
+      <c r="D18" s="5">
+        <v>-23</v>
+      </c>
+      <c r="E18" s="5">
+        <v>-16</v>
+      </c>
+      <c r="F18" s="5">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4">
+        <v>953</v>
+      </c>
+      <c r="C19" s="4">
+        <v>828</v>
+      </c>
+      <c r="D19" s="5">
+        <v>662</v>
+      </c>
+      <c r="E19" s="5">
+        <v>600</v>
+      </c>
+      <c r="F19" s="5">
+        <v>-24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20" s="4">
+        <v>980</v>
+      </c>
+      <c r="C20" s="4">
+        <v>994</v>
+      </c>
+      <c r="D20" s="5">
+        <v>636</v>
+      </c>
+      <c r="E20" s="5">
+        <v>877</v>
+      </c>
+      <c r="F20" s="5">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>19</v>
+      </c>
+      <c r="B21" s="4">
+        <v>957</v>
+      </c>
+      <c r="C21" s="4">
+        <v>972</v>
+      </c>
+      <c r="D21" s="5">
+        <v>500</v>
+      </c>
+      <c r="E21" s="5">
+        <v>-68</v>
+      </c>
+      <c r="F21" s="5">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>20</v>
+      </c>
+      <c r="B22" s="4">
+        <v>981</v>
+      </c>
+      <c r="C22" s="4">
+        <v>890</v>
+      </c>
+      <c r="D22" s="5">
+        <v>784</v>
+      </c>
+      <c r="E22" s="5">
+        <v>420</v>
+      </c>
+      <c r="F22" s="5">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23">
+        <f>AVERAGE(B3:B22)</f>
+        <v>722.2</v>
+      </c>
+      <c r="C23">
+        <f>AVERAGE(C3:C22)</f>
+        <v>607</v>
+      </c>
+      <c r="D23">
+        <f>AVERAGE(D3:D22)</f>
+        <v>609.75</v>
+      </c>
+      <c r="E23">
+        <f>AVERAGE(E3:E22)</f>
+        <v>396.8</v>
+      </c>
+      <c r="F23">
+        <f>AVERAGE(F3:F22)</f>
+        <v>387.95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>